<commit_message>
added 3d model GENERATOR added some calculations in sequence.xlsx
</commit_message>
<xml_diff>
--- a/Documentations/sequence.xlsx
+++ b/Documentations/sequence.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\school\2ndyr\1stsem\emag\generotr\Documentations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{847A12AB-1890-483A-AF66-A1E814D050F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAE5EFBC-A2F4-4A33-B015-C5E03F02D126}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A0CABE93-1CAF-4178-A500-DBCC18B4841B}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="152">
   <si>
     <t>Formulas:</t>
   </si>
@@ -253,13 +253,241 @@
   </si>
   <si>
     <t>purpose</t>
+  </si>
+  <si>
+    <t>Realization:</t>
+  </si>
+  <si>
+    <t>scope and edlimitation</t>
+  </si>
+  <si>
+    <t>choose what seems to work (ferris wheel, motor, motor driver)</t>
+  </si>
+  <si>
+    <t>based on:</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>W</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>total (1 rev)</t>
+  </si>
+  <si>
+    <t>coil slot dimension</t>
+  </si>
+  <si>
+    <t>number of turns</t>
+  </si>
+  <si>
+    <t>in mm</t>
+  </si>
+  <si>
+    <t>in m:</t>
+  </si>
+  <si>
+    <t>1 phase length of coil</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>pl/a</t>
+  </si>
+  <si>
+    <t>Diameter ng wire</t>
+  </si>
+  <si>
+    <t>True volt</t>
+  </si>
+  <si>
+    <t>Battery V</t>
+  </si>
+  <si>
+    <t>B field</t>
+  </si>
+  <si>
+    <t>mew naught</t>
+  </si>
+  <si>
+    <t>unknown</t>
+  </si>
+  <si>
+    <t>resistivty of copper @ 20</t>
+  </si>
+  <si>
+    <t>resistvty of copper @ 50</t>
+  </si>
+  <si>
+    <t>configuration</t>
+  </si>
+  <si>
+    <t>wye</t>
+  </si>
+  <si>
+    <t>Motor Design (video 1):</t>
+  </si>
+  <si>
+    <t>Motor Design (1000kv):</t>
+  </si>
+  <si>
+    <t>1 round edge</t>
+  </si>
+  <si>
+    <t>phases of motor</t>
+  </si>
+  <si>
+    <t>number of stator poles</t>
+  </si>
+  <si>
+    <t>number of turns / slot</t>
+  </si>
+  <si>
+    <t>check if the 0.09ohms is for two phases or just 1 phase</t>
+  </si>
+  <si>
+    <t>Motor design (self):</t>
+  </si>
+  <si>
+    <t>Motor Design (video 2):</t>
+  </si>
+  <si>
+    <t>T_R 2 phase</t>
+  </si>
+  <si>
+    <t>Diameter ng wire (mm)</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>mewnaught * n * current</t>
+  </si>
+  <si>
+    <t>tru volts / total R</t>
+  </si>
+  <si>
+    <t>config * total R</t>
+  </si>
+  <si>
+    <t>H field</t>
+  </si>
+  <si>
+    <t>https://www.toppr.com/guides/physics-formulas/magnetic-field-strength-formula/</t>
+  </si>
+  <si>
+    <t>resisitivty of copper * length of copper wire 1 phase / area of wire</t>
+  </si>
+  <si>
+    <t>((Number of turns / length ))</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=DyN-qjOPLKU</t>
+  </si>
+  <si>
+    <t>motor design video poles stator:rotor (6:4)</t>
+  </si>
+  <si>
+    <t>mean radius</t>
+  </si>
+  <si>
+    <t>NI / radius in m</t>
+  </si>
+  <si>
+    <t>h2 field</t>
+  </si>
+  <si>
+    <t>B2 field</t>
+  </si>
+  <si>
+    <t>mew * H2</t>
+  </si>
+  <si>
+    <t>mew medium</t>
+  </si>
+  <si>
+    <t>mew * n * current</t>
+  </si>
+  <si>
+    <t>mean radius 1phase</t>
+  </si>
+  <si>
+    <t>NI / length per phase</t>
+  </si>
+  <si>
+    <t>h3 field</t>
+  </si>
+  <si>
+    <t>NI / length of slot in m</t>
+  </si>
+  <si>
+    <t>B3 field</t>
+  </si>
+  <si>
+    <t>mew * H3</t>
+  </si>
+  <si>
+    <t>B_H field</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mew * H </t>
+  </si>
+  <si>
+    <t>1 phase length of coil (square)</t>
+  </si>
+  <si>
+    <t>1 phase length of coil (circle)</t>
+  </si>
+  <si>
+    <t>length perphase C m:</t>
+  </si>
+  <si>
+    <t>length perphase S m:</t>
+  </si>
+  <si>
+    <t>NI / radius in m for 1 slot</t>
+  </si>
+  <si>
+    <t>for one phase</t>
+  </si>
+  <si>
+    <t>B_H field2</t>
+  </si>
+  <si>
+    <t>for one slot</t>
+  </si>
+  <si>
+    <t>mew * (NI/L)</t>
+  </si>
+  <si>
+    <t>Force</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S </t>
+  </si>
+  <si>
+    <t>pi * r^2</t>
+  </si>
+  <si>
+    <t>F = {(B_Hfield2^2)   * S   } /  {      2 * mew}</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> for one slot</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -283,16 +511,30 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="7">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -362,12 +604,118 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -379,6 +727,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -694,16 +1063,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F298B35-6B67-4A34-9984-D13A8F00E275}">
-  <dimension ref="C4:V96"/>
+  <dimension ref="C4:AP189"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="E97" sqref="E97"/>
+    <sheetView tabSelected="1" topLeftCell="A147" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G152" sqref="G152"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="22.33203125" customWidth="1"/>
-    <col min="9" max="9" width="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.33203125" customWidth="1"/>
+    <col min="10" max="10" width="11.6640625" customWidth="1"/>
+    <col min="16" max="16" width="12.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="3:22" x14ac:dyDescent="0.3">
@@ -1220,12 +1593,1303 @@
         <v>75</v>
       </c>
     </row>
+    <row r="98" spans="3:37" x14ac:dyDescent="0.3">
+      <c r="C98" s="23" t="s">
+        <v>122</v>
+      </c>
+      <c r="D98" s="1" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="99" spans="3:37" x14ac:dyDescent="0.3">
+      <c r="C99" s="23"/>
+    </row>
+    <row r="102" spans="3:37" x14ac:dyDescent="0.3">
+      <c r="C102" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="103" spans="3:37" x14ac:dyDescent="0.3">
+      <c r="D103" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="104" spans="3:37" x14ac:dyDescent="0.3">
+      <c r="D104">
+        <v>1</v>
+      </c>
+      <c r="E104" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="105" spans="3:37" x14ac:dyDescent="0.3">
+      <c r="D105">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="111" spans="3:37" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C111" t="s">
+        <v>102</v>
+      </c>
+      <c r="M111" t="s">
+        <v>103</v>
+      </c>
+      <c r="AI111" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="112" spans="3:37" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D112" t="s">
+        <v>79</v>
+      </c>
+      <c r="E112" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="N112" t="s">
+        <v>79</v>
+      </c>
+      <c r="O112" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="AJ112" t="s">
+        <v>79</v>
+      </c>
+      <c r="AK112" s="11" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="113" spans="5:42" x14ac:dyDescent="0.3">
+      <c r="G113" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="H113" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="I113" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="J113" s="16" t="s">
+        <v>104</v>
+      </c>
+      <c r="K113" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q113" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="R113" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="S113" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="T113" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="AM113" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="AN113" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="AO113" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="AP113" s="16" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="114" spans="5:42" x14ac:dyDescent="0.3">
+      <c r="E114" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="F114" s="15"/>
+      <c r="G114" s="12">
+        <v>18</v>
+      </c>
+      <c r="H114" s="13">
+        <f>14</f>
+        <v>14</v>
+      </c>
+      <c r="I114" s="12">
+        <v>16</v>
+      </c>
+      <c r="J114" s="12">
+        <f>2*PI()*1/4</f>
+        <v>1.5707963267948966</v>
+      </c>
+      <c r="K114" s="12">
+        <f>(H114*2)+(I114*2)+(J114*4)</f>
+        <v>66.283185307179593</v>
+      </c>
+      <c r="O114" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="P114" s="15"/>
+      <c r="Q114" s="12">
+        <v>5</v>
+      </c>
+      <c r="R114" s="13">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="S114" s="12">
+        <v>1.4</v>
+      </c>
+      <c r="T114" s="12">
+        <f>(R114*2)+(S114*2)</f>
+        <v>3.92</v>
+      </c>
+      <c r="AK114" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="AL114" s="15"/>
+      <c r="AM114" s="12">
+        <v>5</v>
+      </c>
+      <c r="AN114" s="13">
+        <v>0.5</v>
+      </c>
+      <c r="AO114" s="12">
+        <v>1.4</v>
+      </c>
+      <c r="AP114" s="12">
+        <f>(AN114*2)+(AO114*2)</f>
+        <v>3.8</v>
+      </c>
+    </row>
+    <row r="115" spans="5:42" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E115" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="F115" s="15"/>
+      <c r="G115" s="12">
+        <v>100</v>
+      </c>
+      <c r="O115" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="P115" s="15"/>
+      <c r="Q115" s="12">
+        <v>13</v>
+      </c>
+      <c r="AK115" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="AL115" s="15"/>
+      <c r="AM115" s="12">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="116" spans="5:42" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E116" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="F116" s="15"/>
+      <c r="G116" s="12">
+        <f>K114*G115</f>
+        <v>6628.3185307179592</v>
+      </c>
+      <c r="I116" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="J116" s="10">
+        <f>G116/1000</f>
+        <v>6.6283185307179595</v>
+      </c>
+      <c r="O116" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="P116" s="15"/>
+      <c r="Q116" s="12">
+        <f>T114*Q115*(Q117/Q118)</f>
+        <v>203.84</v>
+      </c>
+      <c r="S116" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="T116" s="10">
+        <f>Q116/1000</f>
+        <v>0.20383999999999999</v>
+      </c>
+      <c r="AK116" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="AL116" s="15"/>
+      <c r="AM116" s="12">
+        <f>AP114*AM115*(AM117/AM118)</f>
+        <v>197.6</v>
+      </c>
+      <c r="AO116" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="AP116" s="10">
+        <f>AM116/1000</f>
+        <v>0.1976</v>
+      </c>
+    </row>
+    <row r="117" spans="5:42" x14ac:dyDescent="0.3">
+      <c r="E117" t="s">
+        <v>106</v>
+      </c>
+      <c r="G117">
+        <v>3</v>
+      </c>
+      <c r="I117" t="s">
+        <v>123</v>
+      </c>
+      <c r="J117">
+        <f>K114/(2*PI())</f>
+        <v>10.549296585513721</v>
+      </c>
+      <c r="O117" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="P117" s="15"/>
+      <c r="Q117">
+        <v>12</v>
+      </c>
+      <c r="S117" t="s">
+        <v>123</v>
+      </c>
+      <c r="T117">
+        <f>T114/(2*PI())</f>
+        <v>0.62388737692022977</v>
+      </c>
+      <c r="AK117" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="AL117" s="15"/>
+      <c r="AM117">
+        <v>12</v>
+      </c>
+      <c r="AO117" t="s">
+        <v>123</v>
+      </c>
+      <c r="AP117">
+        <f>AP114/(2*PI())</f>
+        <v>0.60478878374920231</v>
+      </c>
+    </row>
+    <row r="118" spans="5:42" x14ac:dyDescent="0.3">
+      <c r="E118" t="s">
+        <v>105</v>
+      </c>
+      <c r="G118">
+        <v>3</v>
+      </c>
+      <c r="O118" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="P118" s="15"/>
+      <c r="Q118">
+        <v>3</v>
+      </c>
+      <c r="AK118" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="AL118" s="15"/>
+      <c r="AM118">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="119" spans="5:42" x14ac:dyDescent="0.3">
+      <c r="E119" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="F119">
+        <v>2</v>
+      </c>
+      <c r="G119" t="s">
+        <v>101</v>
+      </c>
+      <c r="O119" s="18" t="s">
+        <v>100</v>
+      </c>
+      <c r="P119">
+        <v>2</v>
+      </c>
+      <c r="Q119" t="s">
+        <v>101</v>
+      </c>
+      <c r="AK119" s="18" t="s">
+        <v>100</v>
+      </c>
+      <c r="AL119">
+        <v>2</v>
+      </c>
+      <c r="AM119" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="120" spans="5:42" x14ac:dyDescent="0.3">
+      <c r="E120" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="F120">
+        <v>12</v>
+      </c>
+      <c r="G120" t="s">
+        <v>97</v>
+      </c>
+      <c r="O120" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="P120">
+        <v>12</v>
+      </c>
+      <c r="AK120" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="AL120">
+        <v>12</v>
+      </c>
+      <c r="AM120" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="121" spans="5:42" x14ac:dyDescent="0.3">
+      <c r="E121" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="F121">
+        <v>1.4</v>
+      </c>
+      <c r="G121" t="s">
+        <v>97</v>
+      </c>
+      <c r="O121" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="P121">
+        <v>0</v>
+      </c>
+      <c r="Q121">
+        <v>3.9</v>
+      </c>
+      <c r="AK121" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="AL121">
+        <v>2</v>
+      </c>
+      <c r="AM121" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="122" spans="5:42" x14ac:dyDescent="0.3">
+      <c r="E122" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="F122">
+        <f>F120-F121</f>
+        <v>10.6</v>
+      </c>
+      <c r="G122" t="s">
+        <v>97</v>
+      </c>
+      <c r="O122" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="P122">
+        <f>P120-P121</f>
+        <v>12</v>
+      </c>
+      <c r="AK122" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="AL122">
+        <f>AL120-AL121</f>
+        <v>10</v>
+      </c>
+      <c r="AM122" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="123" spans="5:42" x14ac:dyDescent="0.3">
+      <c r="E123" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="F123">
+        <f>F122/(F125)</f>
+        <v>30.165317682660437</v>
+      </c>
+      <c r="G123" t="s">
+        <v>97</v>
+      </c>
+      <c r="O123" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="P123" s="19">
+        <f>P122/(P125)</f>
+        <v>53.638231573108264</v>
+      </c>
+      <c r="AK123" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="AL123" s="21">
+        <f>AL122/(AL125)</f>
+        <v>46.110058720742195</v>
+      </c>
+      <c r="AM123" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="124" spans="5:42" x14ac:dyDescent="0.3">
+      <c r="E124" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="F124">
+        <f>((G128)    *  (J116)      ) /(PI() * ((G127/2) * (1/1000))^2    )</f>
+        <v>0.17569846456636307</v>
+      </c>
+      <c r="J124" t="s">
+        <v>91</v>
+      </c>
+      <c r="O124" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="P124" s="19">
+        <f>((Q128)    *  (T116)      ) /(PI() * ((Q127/2) * (1/1000))^2    )</f>
+        <v>0.11186051113228952</v>
+      </c>
+      <c r="Q124" s="20" t="s">
+        <v>108</v>
+      </c>
+      <c r="T124" t="s">
+        <v>91</v>
+      </c>
+      <c r="AK124" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="AL124" s="21">
+        <f>((AM128)    *  (AP116)      ) /(PI() * ((AM127/2) * (1/1000))^2    )</f>
+        <v>0.10843620977109697</v>
+      </c>
+      <c r="AM124" s="20"/>
+      <c r="AP124" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="125" spans="5:42" x14ac:dyDescent="0.3">
+      <c r="E125" s="22" t="s">
+        <v>111</v>
+      </c>
+      <c r="F125">
+        <f>F124*F119</f>
+        <v>0.35139692913272613</v>
+      </c>
+      <c r="O125" s="22" t="s">
+        <v>111</v>
+      </c>
+      <c r="P125">
+        <f>P124*P119</f>
+        <v>0.22372102226457904</v>
+      </c>
+      <c r="AK125" s="22" t="s">
+        <v>111</v>
+      </c>
+      <c r="AL125">
+        <f>AL124*AL119</f>
+        <v>0.21687241954219394</v>
+      </c>
+    </row>
+    <row r="127" spans="5:42" x14ac:dyDescent="0.3">
+      <c r="E127" t="s">
+        <v>92</v>
+      </c>
+      <c r="G127">
+        <f>0.91</f>
+        <v>0.91</v>
+      </c>
+      <c r="O127" t="s">
+        <v>92</v>
+      </c>
+      <c r="Q127">
+        <f>0.2</f>
+        <v>0.2</v>
+      </c>
+      <c r="AK127" t="s">
+        <v>92</v>
+      </c>
+      <c r="AM127">
+        <f>0.2</f>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="128" spans="5:42" x14ac:dyDescent="0.3">
+      <c r="E128" t="s">
+        <v>98</v>
+      </c>
+      <c r="G128">
+        <f>1.724*10^-8</f>
+        <v>1.7240000000000001E-8</v>
+      </c>
+      <c r="O128" t="s">
+        <v>98</v>
+      </c>
+      <c r="Q128">
+        <f>1.724*10^-8</f>
+        <v>1.7240000000000001E-8</v>
+      </c>
+      <c r="AK128" t="s">
+        <v>98</v>
+      </c>
+      <c r="AM128">
+        <f>1.724*10^-8</f>
+        <v>1.7240000000000001E-8</v>
+      </c>
+    </row>
+    <row r="129" spans="5:42" x14ac:dyDescent="0.3">
+      <c r="E129" t="s">
+        <v>99</v>
+      </c>
+      <c r="G129">
+        <f>2.43*10^-8</f>
+        <v>2.4300000000000003E-8</v>
+      </c>
+      <c r="O129" t="s">
+        <v>99</v>
+      </c>
+      <c r="Q129">
+        <f>2.43*10^-8</f>
+        <v>2.4300000000000003E-8</v>
+      </c>
+      <c r="AK129" t="s">
+        <v>99</v>
+      </c>
+      <c r="AM129">
+        <f>2.43*10^-8</f>
+        <v>2.4300000000000003E-8</v>
+      </c>
+    </row>
+    <row r="131" spans="5:42" x14ac:dyDescent="0.3">
+      <c r="E131" t="s">
+        <v>95</v>
+      </c>
+      <c r="F131">
+        <f>F132*F137*F133*F123</f>
+        <v>0.21059364538899625</v>
+      </c>
+      <c r="J131" t="s">
+        <v>129</v>
+      </c>
+      <c r="O131" t="s">
+        <v>95</v>
+      </c>
+      <c r="P131" t="e">
+        <f>P132*P138*P133*P123</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T131" t="s">
+        <v>129</v>
+      </c>
+      <c r="W131" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="AK131" t="s">
+        <v>95</v>
+      </c>
+      <c r="AL131">
+        <f>AL132*AL133*AL123</f>
+        <v>0.15065338260302477</v>
+      </c>
+      <c r="AP131" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="132" spans="5:42" x14ac:dyDescent="0.3">
+      <c r="E132" t="s">
+        <v>96</v>
+      </c>
+      <c r="F132">
+        <f>4*PI()*10^-7</f>
+        <v>1.2566370614359173E-6</v>
+      </c>
+      <c r="O132" t="s">
+        <v>96</v>
+      </c>
+      <c r="P132">
+        <f>4*PI()*10^-7</f>
+        <v>1.2566370614359173E-6</v>
+      </c>
+      <c r="AK132" t="s">
+        <v>96</v>
+      </c>
+      <c r="AL132">
+        <f>4*PI()*10^-7</f>
+        <v>1.2566370614359173E-6</v>
+      </c>
+    </row>
+    <row r="133" spans="5:42" x14ac:dyDescent="0.3">
+      <c r="E133" t="s">
+        <v>113</v>
+      </c>
+      <c r="F133">
+        <f>(G115/(G114/1000))</f>
+        <v>5555.5555555555557</v>
+      </c>
+      <c r="J133" t="s">
+        <v>120</v>
+      </c>
+      <c r="O133" t="s">
+        <v>113</v>
+      </c>
+      <c r="P133" t="e">
+        <f>(Q109/(Q108/1000))</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T133" t="s">
+        <v>120</v>
+      </c>
+      <c r="AK133" t="s">
+        <v>113</v>
+      </c>
+      <c r="AL133">
+        <f>(AM115/(AM114/1000))</f>
+        <v>2600</v>
+      </c>
+      <c r="AP133" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="134" spans="5:42" x14ac:dyDescent="0.3">
+      <c r="E134" t="s">
+        <v>126</v>
+      </c>
+      <c r="F134">
+        <f>F132*F137*F141</f>
+        <v>0.35933065169551659</v>
+      </c>
+      <c r="J134" t="s">
+        <v>127</v>
+      </c>
+      <c r="O134" t="s">
+        <v>126</v>
+      </c>
+      <c r="P134" t="e">
+        <f>P132*P138*P145</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T134" t="s">
+        <v>127</v>
+      </c>
+      <c r="AK134" t="s">
+        <v>126</v>
+      </c>
+      <c r="AL134">
+        <f>AL132*AL135*AL138</f>
+        <v>0.12455041053266182</v>
+      </c>
+      <c r="AP134" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="135" spans="5:42" x14ac:dyDescent="0.3">
+      <c r="E135" t="s">
+        <v>134</v>
+      </c>
+      <c r="F135">
+        <f>F132*F137*(G114*10^-3)</f>
+        <v>2.2619467105846513E-8</v>
+      </c>
+      <c r="J135" t="s">
+        <v>135</v>
+      </c>
+      <c r="O135" t="s">
+        <v>134</v>
+      </c>
+      <c r="P135">
+        <f>P132*P138*(Q108*10^-3)</f>
+        <v>0</v>
+      </c>
+      <c r="T135" t="s">
+        <v>135</v>
+      </c>
+      <c r="AK135" t="s">
+        <v>128</v>
+      </c>
+      <c r="AL135">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="136" spans="5:42" x14ac:dyDescent="0.3">
+      <c r="E136" t="s">
+        <v>136</v>
+      </c>
+      <c r="F136">
+        <f>F132*F137*F140</f>
+        <v>5.7189249421773602E-4</v>
+      </c>
+      <c r="J136" t="s">
+        <v>137</v>
+      </c>
+      <c r="O136" t="s">
+        <v>136</v>
+      </c>
+      <c r="P136" t="e">
+        <f>P132*P138*P144</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="T136" t="s">
+        <v>137</v>
+      </c>
+      <c r="U136" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="137" spans="5:42" x14ac:dyDescent="0.3">
+      <c r="E137" t="s">
+        <v>128</v>
+      </c>
+      <c r="F137">
+        <v>1</v>
+      </c>
+      <c r="O137" t="s">
+        <v>144</v>
+      </c>
+      <c r="P137">
+        <f>P132*P138*((Q115*P123)/(Q114/1000))</f>
+        <v>175.24985323209</v>
+      </c>
+      <c r="T137" t="s">
+        <v>146</v>
+      </c>
+      <c r="U137" t="s">
+        <v>145</v>
+      </c>
+      <c r="AK137" t="s">
+        <v>117</v>
+      </c>
+      <c r="AL137">
+        <f>AM115*AL123/AP116</f>
+        <v>3033.5564947856706</v>
+      </c>
+    </row>
+    <row r="138" spans="5:42" x14ac:dyDescent="0.3">
+      <c r="O138" t="s">
+        <v>128</v>
+      </c>
+      <c r="P138">
+        <v>1000</v>
+      </c>
+      <c r="AK138" t="s">
+        <v>125</v>
+      </c>
+      <c r="AL138">
+        <f>AM115*AL123/(AP117*10^-2)</f>
+        <v>99114.067501989965</v>
+      </c>
+      <c r="AP138" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="140" spans="5:42" x14ac:dyDescent="0.3">
+      <c r="E140" t="s">
+        <v>117</v>
+      </c>
+      <c r="F140">
+        <f>G115*F123/J116</f>
+        <v>455.09758685952926</v>
+      </c>
+      <c r="J140" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="141" spans="5:42" x14ac:dyDescent="0.3">
+      <c r="E141" t="s">
+        <v>125</v>
+      </c>
+      <c r="F141">
+        <f>G115*F123/(J117*10^-3)</f>
+        <v>285946.24710886803</v>
+      </c>
+      <c r="J141" t="s">
+        <v>142</v>
+      </c>
+      <c r="O141" t="s">
+        <v>147</v>
+      </c>
+      <c r="P141">
+        <f>((P137^2)*Z141)/(2*P138*P132)</f>
+        <v>0.38390638822336359</v>
+      </c>
+      <c r="T141" t="s">
+        <v>150</v>
+      </c>
+      <c r="X141" t="s">
+        <v>148</v>
+      </c>
+      <c r="Y141" t="s">
+        <v>149</v>
+      </c>
+      <c r="Z141">
+        <f>PI()*(Q127/2000)^2</f>
+        <v>3.1415926535897931E-8</v>
+      </c>
+    </row>
+    <row r="142" spans="5:42" x14ac:dyDescent="0.3">
+      <c r="E142" t="s">
+        <v>132</v>
+      </c>
+      <c r="F142">
+        <f>G116*F124/(G114*10^-3)</f>
+        <v>64699.188250217609</v>
+      </c>
+      <c r="J142" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="144" spans="5:42" x14ac:dyDescent="0.3">
+      <c r="O144" t="s">
+        <v>117</v>
+      </c>
+      <c r="P144" t="e">
+        <f>Q109*(Q113/Q114)*P123/T111</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="T144" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="145" spans="3:20" x14ac:dyDescent="0.3">
+      <c r="O145" t="s">
+        <v>125</v>
+      </c>
+      <c r="P145" t="e">
+        <f>Q109*P123/(T112*10^-3)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T145" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="146" spans="3:20" x14ac:dyDescent="0.3">
+      <c r="O146" t="s">
+        <v>132</v>
+      </c>
+      <c r="P146" t="e">
+        <f>Q111*P124/(Q108*10^-3)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T146" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="148" spans="3:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C148" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="149" spans="3:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D149" t="s">
+        <v>79</v>
+      </c>
+      <c r="E149" s="11" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="150" spans="3:20" x14ac:dyDescent="0.3">
+      <c r="G150" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="H150" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="I150" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="J150" s="16" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="151" spans="3:20" x14ac:dyDescent="0.3">
+      <c r="E151" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="F151" s="17"/>
+      <c r="G151" s="12">
+        <v>10</v>
+      </c>
+      <c r="H151" s="13">
+        <v>3</v>
+      </c>
+      <c r="I151" s="12">
+        <v>3</v>
+      </c>
+      <c r="J151" s="12">
+        <f>(H151*2)+(I151*2)</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="152" spans="3:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E152" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="F152" s="17"/>
+      <c r="G152" s="12">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="153" spans="3:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E153" s="17" t="s">
+        <v>138</v>
+      </c>
+      <c r="F153" s="17"/>
+      <c r="G153" s="12">
+        <f>J151*G152*(G156/G157)</f>
+        <v>1200</v>
+      </c>
+      <c r="I153" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="J153" s="10">
+        <f>G153/1000</f>
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="154" spans="3:20" x14ac:dyDescent="0.3">
+      <c r="D154" t="s">
+        <v>139</v>
+      </c>
+      <c r="G154">
+        <f>(2*PI()*J155*G152) *(G156/G157)</f>
+        <v>6283.1853071795858</v>
+      </c>
+      <c r="I154" t="s">
+        <v>140</v>
+      </c>
+      <c r="J154">
+        <f>G154/1000</f>
+        <v>6.2831853071795862</v>
+      </c>
+    </row>
+    <row r="155" spans="3:20" x14ac:dyDescent="0.3">
+      <c r="I155" t="s">
+        <v>130</v>
+      </c>
+      <c r="J155">
+        <v>10</v>
+      </c>
+      <c r="K155">
+        <f>K151/(2*PI())</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="156" spans="3:20" x14ac:dyDescent="0.3">
+      <c r="E156" s="17" t="s">
+        <v>106</v>
+      </c>
+      <c r="F156" s="17"/>
+      <c r="G156">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="157" spans="3:20" x14ac:dyDescent="0.3">
+      <c r="E157" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="F157" s="17"/>
+      <c r="G157">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="162" spans="5:13" x14ac:dyDescent="0.3">
+      <c r="E162" s="18" t="s">
+        <v>100</v>
+      </c>
+      <c r="F162">
+        <v>2</v>
+      </c>
+      <c r="G162" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="163" spans="5:13" x14ac:dyDescent="0.3">
+      <c r="E163" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="F163">
+        <v>12</v>
+      </c>
+      <c r="G163" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="164" spans="5:13" x14ac:dyDescent="0.3">
+      <c r="E164" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="F164" s="19">
+        <v>0</v>
+      </c>
+      <c r="G164" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="165" spans="5:13" x14ac:dyDescent="0.3">
+      <c r="E165" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="F165">
+        <f>F163-F164</f>
+        <v>12</v>
+      </c>
+      <c r="G165" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="166" spans="5:13" x14ac:dyDescent="0.3">
+      <c r="E166" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="F166" s="21">
+        <f>F165/F168</f>
+        <v>111.61400813942856</v>
+      </c>
+      <c r="G166" t="s">
+        <v>97</v>
+      </c>
+      <c r="J166" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="167" spans="5:13" x14ac:dyDescent="0.3">
+      <c r="E167" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="F167" s="21">
+        <f>((G171)    *  (J153)      ) /(PI() * ((G170/2) * (1/1000))^2    )</f>
+        <v>5.3756693268328666E-2</v>
+      </c>
+      <c r="G167" s="20"/>
+      <c r="J167" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="168" spans="5:13" x14ac:dyDescent="0.3">
+      <c r="E168" s="22" t="s">
+        <v>111</v>
+      </c>
+      <c r="F168">
+        <f>F167*F162</f>
+        <v>0.10751338653665733</v>
+      </c>
+      <c r="J168" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="170" spans="5:13" x14ac:dyDescent="0.3">
+      <c r="E170" t="s">
+        <v>112</v>
+      </c>
+      <c r="G170">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="171" spans="5:13" x14ac:dyDescent="0.3">
+      <c r="E171" t="s">
+        <v>98</v>
+      </c>
+      <c r="G171">
+        <f>1.724*10^-8</f>
+        <v>1.7240000000000001E-8</v>
+      </c>
+    </row>
+    <row r="172" spans="5:13" x14ac:dyDescent="0.3">
+      <c r="E172" t="s">
+        <v>99</v>
+      </c>
+      <c r="G172">
+        <f>2.43*10^-8</f>
+        <v>2.4300000000000003E-8</v>
+      </c>
+    </row>
+    <row r="174" spans="5:13" x14ac:dyDescent="0.3">
+      <c r="E174" t="s">
+        <v>95</v>
+      </c>
+      <c r="F174">
+        <f>F175*F181*F176*F166</f>
+        <v>140.25829920341607</v>
+      </c>
+      <c r="J174" t="s">
+        <v>129</v>
+      </c>
+      <c r="M174" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="175" spans="5:13" x14ac:dyDescent="0.3">
+      <c r="E175" t="s">
+        <v>96</v>
+      </c>
+      <c r="F175">
+        <f>4*PI()*10^-7</f>
+        <v>1.2566370614359173E-6</v>
+      </c>
+    </row>
+    <row r="176" spans="5:13" x14ac:dyDescent="0.3">
+      <c r="E176" t="s">
+        <v>113</v>
+      </c>
+      <c r="F176">
+        <f>(G152/(G151/1000))</f>
+        <v>10000</v>
+      </c>
+      <c r="J176" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="177" spans="5:11" x14ac:dyDescent="0.3">
+      <c r="E177" t="s">
+        <v>126</v>
+      </c>
+      <c r="F177">
+        <f>F175*F181*F188</f>
+        <v>140.25829920341607</v>
+      </c>
+      <c r="J177" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="178" spans="5:11" x14ac:dyDescent="0.3">
+      <c r="E178" t="s">
+        <v>134</v>
+      </c>
+      <c r="F178">
+        <f>F175*F181*(G151*10^-2)</f>
+        <v>1.2566370614359175E-5</v>
+      </c>
+      <c r="J178" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="179" spans="5:11" x14ac:dyDescent="0.3">
+      <c r="E179" t="s">
+        <v>136</v>
+      </c>
+      <c r="F179">
+        <f>F175*F181*F187</f>
+        <v>0.22322801627885716</v>
+      </c>
+      <c r="J179" t="s">
+        <v>137</v>
+      </c>
+      <c r="K179" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="180" spans="5:11" x14ac:dyDescent="0.3">
+      <c r="E180" t="s">
+        <v>144</v>
+      </c>
+      <c r="F180">
+        <f>F175*F181*((G152*F166)/(G151/1000))</f>
+        <v>140.25829920341607</v>
+      </c>
+      <c r="J180" t="s">
+        <v>146</v>
+      </c>
+      <c r="K180" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="181" spans="5:11" x14ac:dyDescent="0.3">
+      <c r="E181" t="s">
+        <v>128</v>
+      </c>
+      <c r="F181">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="183" spans="5:11" x14ac:dyDescent="0.3">
+      <c r="E183" t="s">
+        <v>148</v>
+      </c>
+      <c r="F183">
+        <f>PI()*(G170/2000)^2</f>
+        <v>3.8484510006474966E-7</v>
+      </c>
+      <c r="J183" t="s">
+        <v>149</v>
+      </c>
+      <c r="K183" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="184" spans="5:11" x14ac:dyDescent="0.3">
+      <c r="E184" t="s">
+        <v>147</v>
+      </c>
+      <c r="F184">
+        <f>((F180^2)*F183)/(2*F181*F175)</f>
+        <v>30.123347946134817</v>
+      </c>
+      <c r="J184" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="187" spans="5:11" x14ac:dyDescent="0.3">
+      <c r="E187" t="s">
+        <v>117</v>
+      </c>
+      <c r="F187">
+        <f>G152*(G156/G157)*F166/J154</f>
+        <v>1776.3921113689098</v>
+      </c>
+      <c r="J187" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="188" spans="5:11" x14ac:dyDescent="0.3">
+      <c r="E188" t="s">
+        <v>125</v>
+      </c>
+      <c r="F188">
+        <f>G152*F166/(J155*10^-3)</f>
+        <v>1116140.0813942857</v>
+      </c>
+      <c r="J188" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="189" spans="5:11" x14ac:dyDescent="0.3">
+      <c r="E189" t="s">
+        <v>132</v>
+      </c>
+      <c r="F189">
+        <f>G154*F167/(G151*10^-3)</f>
+        <v>33776.326530612241</v>
+      </c>
+      <c r="J189" t="s">
+        <v>133</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="14">
+    <mergeCell ref="C98:C99"/>
+    <mergeCell ref="O117:P117"/>
+    <mergeCell ref="O118:P118"/>
+    <mergeCell ref="AK114:AL114"/>
+    <mergeCell ref="AK115:AL115"/>
+    <mergeCell ref="AK116:AL116"/>
+    <mergeCell ref="AK117:AL117"/>
+    <mergeCell ref="AK118:AL118"/>
+    <mergeCell ref="E116:F116"/>
+    <mergeCell ref="E115:F115"/>
+    <mergeCell ref="E114:F114"/>
+    <mergeCell ref="O114:P114"/>
+    <mergeCell ref="O115:P115"/>
+    <mergeCell ref="O116:P116"/>
+  </mergeCells>
   <hyperlinks>
     <hyperlink ref="V6" r:id="rId1" xr:uid="{ABC3A435-B1B5-4ADE-8995-32B666B52930}"/>
     <hyperlink ref="D45" r:id="rId2" xr:uid="{30279D9E-C0C7-4DB1-B524-56F0E43E6352}"/>
     <hyperlink ref="E87" r:id="rId3" xr:uid="{B3FD3783-F41D-4BFF-B225-62C91710B70D}"/>
     <hyperlink ref="E88" r:id="rId4" xr:uid="{76FD13A0-29B1-4AD4-B9A9-8325770F6864}"/>
+    <hyperlink ref="M174" r:id="rId5" xr:uid="{79751D78-4AEC-44DE-AC1E-BA8958ECC5B8}"/>
+    <hyperlink ref="D98" r:id="rId6" xr:uid="{B7D8395C-6009-4E53-8ACA-509F289CCAF3}"/>
+    <hyperlink ref="W131" r:id="rId7" xr:uid="{9A1BFDCD-A14D-44F9-B3A7-1B4DD4B5B216}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
revision of 3d model
</commit_message>
<xml_diff>
--- a/Documentations/sequence.xlsx
+++ b/Documentations/sequence.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\school\2ndyr\1stsem\emag\generotr\Documentations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44A97773-7161-4518-A2F6-87333D51C2F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B12B96E-EEE0-43BF-8232-FCCCBFC9DF18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A0CABE93-1CAF-4178-A500-DBCC18B4841B}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="521" uniqueCount="174">
   <si>
     <t>Formulas:</t>
   </si>
@@ -354,9 +354,6 @@
     <t>check if the 0.09ohms is for two phases or just 1 phase</t>
   </si>
   <si>
-    <t>Motor design (self):</t>
-  </si>
-  <si>
     <t>Motor Design (video 2):</t>
   </si>
   <si>
@@ -481,13 +478,111 @@
   </si>
   <si>
     <t xml:space="preserve"> for one slot</t>
+  </si>
+  <si>
+    <t>Motor design (self:: 0.66mm radius):</t>
+  </si>
+  <si>
+    <t>Motor design (self: 0.7 dia):</t>
+  </si>
+  <si>
+    <t>Motor design (self: 0.7 dia, n42 magnet):</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.scribd.com/document/427205752/American-Wire-Gauge-Conductor-Size-Table-pdf </t>
+  </si>
+  <si>
+    <t>0.7 mm dia (ampacity=    ~1A)</t>
+  </si>
+  <si>
+    <t>https://www.powerstream.com/Wire_Size.htm</t>
+  </si>
+  <si>
+    <t>0.1mm dia (~0.091A)</t>
+  </si>
+  <si>
+    <t>ratio(dia)</t>
+  </si>
+  <si>
+    <t>ratio(A)</t>
+  </si>
+  <si>
+    <t>ratio ampacity(I : I_allow)</t>
+  </si>
+  <si>
+    <t>allowable current for dia:</t>
+  </si>
+  <si>
+    <t>https://www.rcgroups.com/forums/showthread.php?587549-Motor-formulas</t>
+  </si>
+  <si>
+    <t>Doubling the number of winds halves Kv (rpm/volt) and doubles Kt (torque/Ampere)</t>
+  </si>
+  <si>
+    <t>Doubling statorheight halves Kv, doubles Kt and (roughly) doubles maximum power.</t>
+  </si>
+  <si>
+    <t>https://electronics.stackexchange.com/questions/390683/motor-current-consumption-and-power-do-not-match</t>
+  </si>
+  <si>
+    <r>
+      <t>mechanical output power (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12.75"/>
+        <color theme="1"/>
+        <rFont val="MathJax_Main"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12.75"/>
+        <color theme="1"/>
+        <rFont val="MathJax_Math"/>
+      </rPr>
+      <t>πnT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>).</t>
+    </r>
+  </si>
+  <si>
+    <t>https://www.machinedesign.com/mechanical-motion-systems/article/21251043/portescap-understanding-losses-in-bldc-motors</t>
+  </si>
+  <si>
+    <t>energy losses</t>
+  </si>
+  <si>
+    <t>constant</t>
+  </si>
+  <si>
+    <t>Motor design (very long height):</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=PfjFsSs8qJU</t>
+  </si>
+  <si>
+    <t>Rotor diameter: mm</t>
+  </si>
+  <si>
+    <t>(origin) from rotor radius to stator radius:</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -519,6 +614,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12.75"/>
+      <color theme="1"/>
+      <name val="MathJax_Main"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12.75"/>
+      <color theme="1"/>
+      <name val="MathJax_Math"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="22"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -534,7 +648,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -710,12 +824,49 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -746,6 +897,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1061,13 +1219,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F298B35-6B67-4A34-9984-D13A8F00E275}">
-  <dimension ref="C4:AP189"/>
+  <dimension ref="C4:BL259"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A115" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="P122" sqref="P122"/>
+    <sheetView tabSelected="1" topLeftCell="A96" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="P106" sqref="P106"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="3" max="3" width="22.33203125" customWidth="1"/>
     <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
@@ -1075,19 +1233,22 @@
     <col min="9" max="9" width="17.33203125" customWidth="1"/>
     <col min="10" max="10" width="11.6640625" customWidth="1"/>
     <col min="16" max="16" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="16" customWidth="1"/>
+    <col min="29" max="29" width="14.88671875" customWidth="1"/>
+    <col min="30" max="30" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:22" x14ac:dyDescent="0.3">
+    <row r="4" spans="3:22">
       <c r="C4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="3:22" x14ac:dyDescent="0.3">
+    <row r="5" spans="3:22">
       <c r="D5" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="3:22" x14ac:dyDescent="0.3">
+    <row r="6" spans="3:22">
       <c r="D6" t="s">
         <v>18</v>
       </c>
@@ -1101,12 +1262,12 @@
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="3:6">
       <c r="C19" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="3:6">
       <c r="C21" t="s">
         <v>8</v>
       </c>
@@ -1114,7 +1275,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="3:6">
       <c r="C22" t="s">
         <v>13</v>
       </c>
@@ -1122,7 +1283,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="23" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="3:6">
       <c r="C23" t="s">
         <v>1</v>
       </c>
@@ -1130,27 +1291,27 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="3:6">
       <c r="D24" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="3:6">
       <c r="D25" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="28" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="3:6">
       <c r="C28" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="3:6">
       <c r="D29" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="3:6">
       <c r="E30">
         <v>1</v>
       </c>
@@ -1158,7 +1319,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="3:6">
       <c r="E31">
         <v>2</v>
       </c>
@@ -1166,7 +1327,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="3:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="3:6">
       <c r="E32">
         <v>3</v>
       </c>
@@ -1174,7 +1335,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="33" spans="3:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="3:11">
       <c r="E33">
         <v>4</v>
       </c>
@@ -1182,12 +1343,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="3:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="3:11">
       <c r="D35" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="36" spans="3:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="3:11">
       <c r="E36" t="s">
         <v>11</v>
       </c>
@@ -1198,7 +1359,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="37" spans="3:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="3:11">
       <c r="E37" t="s">
         <v>12</v>
       </c>
@@ -1209,7 +1370,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="38" spans="3:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="3:11">
       <c r="E38" t="s">
         <v>26</v>
       </c>
@@ -1227,7 +1388,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="39" spans="3:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="3:11">
       <c r="E39" t="s">
         <v>28</v>
       </c>
@@ -1236,12 +1397,12 @@
         <v>2.0943951023931953</v>
       </c>
     </row>
-    <row r="44" spans="3:11" x14ac:dyDescent="0.3">
+    <row r="44" spans="3:11">
       <c r="C44" s="8" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="45" spans="3:11" x14ac:dyDescent="0.3">
+    <row r="45" spans="3:11">
       <c r="C45" t="s">
         <v>48</v>
       </c>
@@ -1249,7 +1410,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="46" spans="3:11" x14ac:dyDescent="0.3">
+    <row r="46" spans="3:11">
       <c r="C46" t="s">
         <v>29</v>
       </c>
@@ -1261,7 +1422,7 @@
         <v>0.18</v>
       </c>
     </row>
-    <row r="47" spans="3:11" x14ac:dyDescent="0.3">
+    <row r="47" spans="3:11">
       <c r="C47" t="s">
         <v>55</v>
       </c>
@@ -1273,7 +1434,7 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="48" spans="3:11" x14ac:dyDescent="0.3">
+    <row r="48" spans="3:11">
       <c r="C48" t="s">
         <v>33</v>
       </c>
@@ -1290,7 +1451,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="49" spans="3:11" x14ac:dyDescent="0.3">
+    <row r="49" spans="3:11">
       <c r="C49" t="s">
         <v>34</v>
       </c>
@@ -1304,7 +1465,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="50" spans="3:11" x14ac:dyDescent="0.3">
+    <row r="50" spans="3:11">
       <c r="C50" t="s">
         <v>52</v>
       </c>
@@ -1319,12 +1480,12 @@
         <v>51</v>
       </c>
     </row>
-    <row r="52" spans="3:11" x14ac:dyDescent="0.3">
+    <row r="52" spans="3:11">
       <c r="C52" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="53" spans="3:11" x14ac:dyDescent="0.3">
+    <row r="53" spans="3:11">
       <c r="D53" t="s">
         <v>37</v>
       </c>
@@ -1338,7 +1499,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="54" spans="3:11" x14ac:dyDescent="0.3">
+    <row r="54" spans="3:11">
       <c r="D54" t="s">
         <v>39</v>
       </c>
@@ -1352,7 +1513,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="55" spans="3:11" x14ac:dyDescent="0.3">
+    <row r="55" spans="3:11">
       <c r="D55" t="s">
         <v>41</v>
       </c>
@@ -1364,7 +1525,7 @@
         <v>1.742E-8</v>
       </c>
     </row>
-    <row r="56" spans="3:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="3:11" ht="15" thickBot="1">
       <c r="D56" t="s">
         <v>42</v>
       </c>
@@ -1379,7 +1540,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="57" spans="3:11" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="57" spans="3:11" ht="43.2">
       <c r="C57" s="2" t="s">
         <v>46</v>
       </c>
@@ -1400,7 +1561,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="58" spans="3:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="3:11" ht="15" thickBot="1">
       <c r="C58" s="5" t="s">
         <v>47</v>
       </c>
@@ -1412,12 +1573,12 @@
       <c r="I58" s="6"/>
       <c r="J58" s="7"/>
     </row>
-    <row r="64" spans="3:11" x14ac:dyDescent="0.3">
+    <row r="64" spans="3:11">
       <c r="C64" s="8" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="65" spans="3:11" x14ac:dyDescent="0.3">
+    <row r="65" spans="3:11">
       <c r="C65" t="s">
         <v>54</v>
       </c>
@@ -1428,7 +1589,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="66" spans="3:11" x14ac:dyDescent="0.3">
+    <row r="66" spans="3:11">
       <c r="C66" t="s">
         <v>55</v>
       </c>
@@ -1439,7 +1600,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="67" spans="3:11" x14ac:dyDescent="0.3">
+    <row r="67" spans="3:11">
       <c r="C67" t="s">
         <v>33</v>
       </c>
@@ -1456,7 +1617,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="68" spans="3:11" x14ac:dyDescent="0.3">
+    <row r="68" spans="3:11">
       <c r="C68" t="s">
         <v>34</v>
       </c>
@@ -1470,7 +1631,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="69" spans="3:11" x14ac:dyDescent="0.3">
+    <row r="69" spans="3:11">
       <c r="C69" t="s">
         <v>35</v>
       </c>
@@ -1481,7 +1642,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="75" spans="3:11" x14ac:dyDescent="0.3">
+    <row r="75" spans="3:11">
       <c r="C75" s="8" t="s">
         <v>44</v>
       </c>
@@ -1489,37 +1650,37 @@
         <v>45</v>
       </c>
     </row>
-    <row r="77" spans="3:11" x14ac:dyDescent="0.3">
+    <row r="77" spans="3:11">
       <c r="D77" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="78" spans="3:11" x14ac:dyDescent="0.3">
+    <row r="78" spans="3:11">
       <c r="D78" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="80" spans="3:11" x14ac:dyDescent="0.3">
+    <row r="80" spans="3:11">
       <c r="D80" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="81" spans="4:8" x14ac:dyDescent="0.3">
+    <row r="81" spans="4:8">
       <c r="D81" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="83" spans="4:8" x14ac:dyDescent="0.3">
+    <row r="83" spans="4:8">
       <c r="D83" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="84" spans="4:8" x14ac:dyDescent="0.3">
+    <row r="84" spans="4:8">
       <c r="D84" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="86" spans="4:8" x14ac:dyDescent="0.3">
+    <row r="86" spans="4:8">
       <c r="E86" t="s">
         <v>62</v>
       </c>
@@ -1533,7 +1694,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="87" spans="4:8" x14ac:dyDescent="0.3">
+    <row r="87" spans="4:8">
       <c r="E87" s="1" t="s">
         <v>63</v>
       </c>
@@ -1548,7 +1709,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="88" spans="4:8" x14ac:dyDescent="0.3">
+    <row r="88" spans="4:8">
       <c r="E88" s="1" t="s">
         <v>68</v>
       </c>
@@ -1563,27 +1724,27 @@
         <v>108</v>
       </c>
     </row>
-    <row r="91" spans="4:8" x14ac:dyDescent="0.3">
+    <row r="91" spans="4:8">
       <c r="D91" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="92" spans="4:8" x14ac:dyDescent="0.3">
+    <row r="92" spans="4:8">
       <c r="D92" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="94" spans="4:8" x14ac:dyDescent="0.3">
+    <row r="94" spans="4:8">
       <c r="D94" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="95" spans="4:8" x14ac:dyDescent="0.3">
+    <row r="95" spans="4:8">
       <c r="D95" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="96" spans="4:8" x14ac:dyDescent="0.3">
+    <row r="96" spans="4:8">
       <c r="E96" t="s">
         <v>65</v>
       </c>
@@ -1591,28 +1752,28 @@
         <v>75</v>
       </c>
     </row>
-    <row r="98" spans="3:37" x14ac:dyDescent="0.3">
+    <row r="98" spans="3:50">
       <c r="C98" s="20" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="99" spans="3:37" x14ac:dyDescent="0.3">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="99" spans="3:50">
       <c r="C99" s="20"/>
     </row>
-    <row r="102" spans="3:37" x14ac:dyDescent="0.3">
+    <row r="102" spans="3:50">
       <c r="C102" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="103" spans="3:37" x14ac:dyDescent="0.3">
+    <row r="103" spans="3:50">
       <c r="D103" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="104" spans="3:37" x14ac:dyDescent="0.3">
+    <row r="104" spans="3:50">
       <c r="D104">
         <v>1</v>
       </c>
@@ -1620,12 +1781,28 @@
         <v>78</v>
       </c>
     </row>
-    <row r="105" spans="3:37" x14ac:dyDescent="0.3">
+    <row r="105" spans="3:50">
       <c r="D105">
         <v>2</v>
       </c>
     </row>
-    <row r="111" spans="3:37" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="106" spans="3:50" ht="28.8">
+      <c r="C106" s="26" t="s">
+        <v>172</v>
+      </c>
+      <c r="F106" s="26">
+        <v>21.5</v>
+      </c>
+    </row>
+    <row r="107" spans="3:50">
+      <c r="C107" t="s">
+        <v>173</v>
+      </c>
+      <c r="F107">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="111" spans="3:50" ht="15" thickBot="1">
       <c r="C111" t="s">
         <v>102</v>
       </c>
@@ -1633,10 +1810,13 @@
         <v>103</v>
       </c>
       <c r="AI111" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="112" spans="3:37" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>109</v>
+      </c>
+      <c r="AX111" s="1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="112" spans="3:50" ht="15" thickBot="1">
       <c r="D112" t="s">
         <v>79</v>
       </c>
@@ -1655,8 +1835,11 @@
       <c r="AK112" s="11" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="113" spans="5:42" x14ac:dyDescent="0.3">
+      <c r="AX112" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="113" spans="5:61" ht="15" thickBot="1">
       <c r="G113" s="14" t="s">
         <v>80</v>
       </c>
@@ -1696,8 +1879,14 @@
       <c r="AP113" s="12" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="114" spans="5:42" x14ac:dyDescent="0.3">
+      <c r="AY113" t="s">
+        <v>79</v>
+      </c>
+      <c r="AZ113" s="11" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="114" spans="5:61">
       <c r="E114" s="21" t="s">
         <v>84</v>
       </c>
@@ -1754,8 +1943,20 @@
         <f>(AN114*2)+(AO114*2)</f>
         <v>3.8</v>
       </c>
-    </row>
-    <row r="115" spans="5:42" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="BB114" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="BC114" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="BD114" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="BE114" s="12" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="115" spans="5:61" ht="15" thickBot="1">
       <c r="E115" s="21" t="s">
         <v>85</v>
       </c>
@@ -1777,8 +1978,29 @@
       <c r="AM115" s="12">
         <v>13</v>
       </c>
-    </row>
-    <row r="116" spans="5:42" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AZ115" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="BA115" s="15"/>
+      <c r="BB115" s="12">
+        <v>10</v>
+      </c>
+      <c r="BC115" s="13">
+        <v>6</v>
+      </c>
+      <c r="BD115" s="12">
+        <v>60</v>
+      </c>
+      <c r="BE115" s="12">
+        <f>(BC115*2)+(BD115*2)</f>
+        <v>132</v>
+      </c>
+      <c r="BG115">
+        <f>((BC115+BC115+BD115+BD115)*BB118)   +( BB118*  (BC115+BB134+BC115+BB134+BD115+BB134+BB134+BD115))   +   (BB118*      (2*(BC115+BB134*3)) +(2*(BD115+BB134*3)))</f>
+        <v>1764.1333333333332</v>
+      </c>
+    </row>
+    <row r="116" spans="5:61" ht="15" thickBot="1">
       <c r="E116" s="21" t="s">
         <v>88</v>
       </c>
@@ -1824,8 +2046,15 @@
         <f>AM116/1000</f>
         <v>0.1976</v>
       </c>
-    </row>
-    <row r="117" spans="5:42" x14ac:dyDescent="0.3">
+      <c r="AZ116" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="BA116" s="15"/>
+      <c r="BB116" s="12">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="117" spans="5:61" ht="15" thickBot="1">
       <c r="E117" t="s">
         <v>106</v>
       </c>
@@ -1833,7 +2062,7 @@
         <v>3</v>
       </c>
       <c r="I117" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="J117">
         <f>K114/(2*PI())</f>
@@ -1847,7 +2076,7 @@
         <v>12</v>
       </c>
       <c r="S117" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="T117">
         <f>T114/(2*PI())</f>
@@ -1861,14 +2090,33 @@
         <v>12</v>
       </c>
       <c r="AO117" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="AP117">
         <f>AP114/(2*PI())</f>
         <v>0.60478878374920231</v>
       </c>
-    </row>
-    <row r="118" spans="5:42" x14ac:dyDescent="0.3">
+      <c r="AZ117" s="15" t="s">
+        <v>137</v>
+      </c>
+      <c r="BA117" s="15"/>
+      <c r="BB117" s="12">
+        <f>BE115*BB116*(BB120/BB121)</f>
+        <v>6600</v>
+      </c>
+      <c r="BD117" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="BE117" s="10">
+        <f>BB117/1000</f>
+        <v>6.6</v>
+      </c>
+      <c r="BG117">
+        <f>BG115/1000</f>
+        <v>1.7641333333333331</v>
+      </c>
+    </row>
+    <row r="118" spans="5:61">
       <c r="E118" t="s">
         <v>105</v>
       </c>
@@ -1889,8 +2137,15 @@
       <c r="AM118">
         <v>3</v>
       </c>
-    </row>
-    <row r="119" spans="5:42" x14ac:dyDescent="0.3">
+      <c r="AZ118" s="25" t="s">
+        <v>169</v>
+      </c>
+      <c r="BB118">
+        <f>BB115/BB134</f>
+        <v>5.5555555555555554</v>
+      </c>
+    </row>
+    <row r="119" spans="5:61">
       <c r="E119" s="12" t="s">
         <v>100</v>
       </c>
@@ -1919,7 +2174,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="120" spans="5:42" x14ac:dyDescent="0.3">
+    <row r="120" spans="5:61" ht="15" thickBot="1">
       <c r="E120" s="12" t="s">
         <v>94</v>
       </c>
@@ -1935,6 +2190,12 @@
       <c r="P120">
         <v>11.82</v>
       </c>
+      <c r="V120" t="s">
+        <v>161</v>
+      </c>
+      <c r="Y120">
+        <v>9.0999999999999998E-2</v>
+      </c>
       <c r="AK120" s="12" t="s">
         <v>94</v>
       </c>
@@ -1944,8 +2205,21 @@
       <c r="AM120" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="121" spans="5:42" x14ac:dyDescent="0.3">
+      <c r="AZ120" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="BA120" s="15"/>
+      <c r="BB120">
+        <v>3</v>
+      </c>
+      <c r="BF120" t="s">
+        <v>161</v>
+      </c>
+      <c r="BI120">
+        <v>7.4</v>
+      </c>
+    </row>
+    <row r="121" spans="5:61" ht="15" thickBot="1">
       <c r="E121" s="12" t="s">
         <v>35</v>
       </c>
@@ -1964,6 +2238,15 @@
       <c r="Q121">
         <v>3.9</v>
       </c>
+      <c r="V121" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="W121" s="24"/>
+      <c r="X121" s="24"/>
+      <c r="Y121" s="10">
+        <f>P123/Y120</f>
+        <v>530.48800456920264</v>
+      </c>
       <c r="AK121" s="12" t="s">
         <v>35</v>
       </c>
@@ -1973,8 +2256,24 @@
       <c r="AM121" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="122" spans="5:42" x14ac:dyDescent="0.3">
+      <c r="AZ121" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="BA121" s="15"/>
+      <c r="BB121">
+        <v>3</v>
+      </c>
+      <c r="BF121" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="BG121" s="24"/>
+      <c r="BH121" s="24"/>
+      <c r="BI121" s="10">
+        <f>BA130/BI120</f>
+        <v>67.83998679132344</v>
+      </c>
+    </row>
+    <row r="122" spans="5:61">
       <c r="E122" s="12" t="s">
         <v>93</v>
       </c>
@@ -2003,7 +2302,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="123" spans="5:42" x14ac:dyDescent="0.3">
+    <row r="123" spans="5:61">
       <c r="E123" s="12" t="s">
         <v>89</v>
       </c>
@@ -2032,7 +2331,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="124" spans="5:42" x14ac:dyDescent="0.3">
+    <row r="124" spans="5:61">
       <c r="E124" s="12" t="s">
         <v>90</v>
       </c>
@@ -2068,30 +2367,41 @@
         <v>91</v>
       </c>
     </row>
-    <row r="125" spans="5:42" x14ac:dyDescent="0.3">
+    <row r="125" spans="5:61">
       <c r="E125" s="19" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F125">
         <f>F124*F119</f>
         <v>0.35139692913272613</v>
       </c>
       <c r="O125" s="19" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="P125">
         <f>P124*P119</f>
         <v>0.22372102226457904</v>
       </c>
       <c r="AK125" s="19" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="AL125">
         <f>AL124*AL119</f>
         <v>0.21687241954219394</v>
       </c>
     </row>
-    <row r="127" spans="5:42" x14ac:dyDescent="0.3">
+    <row r="126" spans="5:61">
+      <c r="AZ126" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="BA126">
+        <v>2</v>
+      </c>
+      <c r="BB126" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="127" spans="5:61">
       <c r="E127" t="s">
         <v>92</v>
       </c>
@@ -2113,8 +2423,17 @@
         <f>0.2</f>
         <v>0.2</v>
       </c>
-    </row>
-    <row r="128" spans="5:42" x14ac:dyDescent="0.3">
+      <c r="AZ127" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="BA127">
+        <v>12</v>
+      </c>
+      <c r="BB127" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="128" spans="5:61">
       <c r="E128" t="s">
         <v>98</v>
       </c>
@@ -2136,8 +2455,17 @@
         <f>1.724*10^-8</f>
         <v>1.7240000000000001E-8</v>
       </c>
-    </row>
-    <row r="129" spans="5:42" x14ac:dyDescent="0.3">
+      <c r="AZ128" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="BA128" s="17">
+        <v>0</v>
+      </c>
+      <c r="BB128" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="129" spans="5:64">
       <c r="E129" t="s">
         <v>99</v>
       </c>
@@ -2159,8 +2487,33 @@
         <f>2.43*10^-8</f>
         <v>2.4300000000000003E-8</v>
       </c>
-    </row>
-    <row r="131" spans="5:42" x14ac:dyDescent="0.3">
+      <c r="AZ129" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="BA129">
+        <f>BA127-BA128</f>
+        <v>12</v>
+      </c>
+      <c r="BB129" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="130" spans="5:64">
+      <c r="AZ130" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="BA130">
+        <f>BA129/BA132</f>
+        <v>502.01590225579349</v>
+      </c>
+      <c r="BB130" t="s">
+        <v>97</v>
+      </c>
+      <c r="BE130" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="131" spans="5:64">
       <c r="E131" t="s">
         <v>95</v>
       </c>
@@ -2169,20 +2522,20 @@
         <v>0.21059364538899625</v>
       </c>
       <c r="J131" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="O131" t="s">
         <v>95</v>
       </c>
-      <c r="P131" t="e">
+      <c r="P131">
         <f>P132*P138*P133*P123</f>
-        <v>#DIV/0!</v>
+        <v>951.20228031202112</v>
       </c>
       <c r="T131" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="W131" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="AK131" t="s">
         <v>95</v>
@@ -2192,10 +2545,21 @@
         <v>0.15065338260302477</v>
       </c>
       <c r="AP131" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="132" spans="5:42" x14ac:dyDescent="0.3">
+        <v>113</v>
+      </c>
+      <c r="AZ131" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="BA131">
+        <f>((BB135)    *  (BG117)      ) /(PI() * ((BB134/2) * (1/1000))^2    )</f>
+        <v>1.195181262792509E-2</v>
+      </c>
+      <c r="BB131" s="18"/>
+      <c r="BE131" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="132" spans="5:64">
       <c r="E132" t="s">
         <v>96</v>
       </c>
@@ -2217,276 +2581,472 @@
         <f>4*PI()*10^-7</f>
         <v>1.2566370614359173E-6</v>
       </c>
-    </row>
-    <row r="133" spans="5:42" x14ac:dyDescent="0.3">
+      <c r="AZ132" s="19" t="s">
+        <v>110</v>
+      </c>
+      <c r="BA132">
+        <f>BA131*BA126</f>
+        <v>2.3903625255850179E-2</v>
+      </c>
+      <c r="BE132" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="133" spans="5:64" ht="15" thickBot="1">
       <c r="E133" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F133">
         <f>(G115/(G114/1000))</f>
         <v>5555.5555555555557</v>
       </c>
       <c r="J133" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="O133" t="s">
-        <v>113</v>
-      </c>
-      <c r="P133" t="e">
-        <f>(Q109/(Q108/1000))</f>
-        <v>#DIV/0!</v>
+        <v>112</v>
+      </c>
+      <c r="P133">
+        <f>(Q116/(Q115/1000))</f>
+        <v>15680.000000000002</v>
       </c>
       <c r="T133" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="AK133" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="AL133">
         <f>(AM115/(AM114/1000))</f>
         <v>2600</v>
       </c>
       <c r="AP133" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="134" spans="5:42" x14ac:dyDescent="0.3">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="134" spans="5:64">
       <c r="E134" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F134">
         <f>F132*F137*F141</f>
         <v>0.35933065169551659</v>
       </c>
       <c r="J134" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="O134" t="s">
+        <v>125</v>
+      </c>
+      <c r="P134">
+        <f>P132*P138*P145</f>
+        <v>157.72486790888101</v>
+      </c>
+      <c r="T134" t="s">
         <v>126</v>
       </c>
-      <c r="P134" t="e">
-        <f>P132*P138*P145</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="T134" t="s">
-        <v>127</v>
-      </c>
       <c r="AK134" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="AL134">
         <f>AL132*AL135*AL138</f>
         <v>0.12455041053266182</v>
       </c>
       <c r="AP134" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="135" spans="5:42" x14ac:dyDescent="0.3">
+        <v>126</v>
+      </c>
+      <c r="AZ134" t="s">
+        <v>111</v>
+      </c>
+      <c r="BB134">
+        <v>1.8</v>
+      </c>
+      <c r="BE134" t="s">
+        <v>158</v>
+      </c>
+      <c r="BF134">
+        <v>0.7</v>
+      </c>
+      <c r="BG134">
+        <v>0.1</v>
+      </c>
+      <c r="BH134" s="22">
+        <f>BF134/BG134</f>
+        <v>6.9999999999999991</v>
+      </c>
+      <c r="BI134" t="s">
+        <v>155</v>
+      </c>
+      <c r="BL134" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="135" spans="5:64" ht="15" thickBot="1">
       <c r="E135" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F135">
         <f>F132*F137*(G114*10^-3)</f>
         <v>2.2619467105846513E-8</v>
       </c>
       <c r="J135" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="O135" t="s">
+        <v>133</v>
+      </c>
+      <c r="P135">
+        <f>P132*P138*(P146*10^-3)</f>
+        <v>0.15772486790888102</v>
+      </c>
+      <c r="T135" t="s">
         <v>134</v>
       </c>
-      <c r="P135">
-        <f>P132*P138*(Q108*10^-3)</f>
-        <v>0</v>
-      </c>
-      <c r="T135" t="s">
-        <v>135</v>
-      </c>
       <c r="AK135" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="AL135">
         <v>1</v>
       </c>
-    </row>
-    <row r="136" spans="5:42" x14ac:dyDescent="0.3">
+      <c r="AZ135" t="s">
+        <v>98</v>
+      </c>
+      <c r="BB135">
+        <f>1.724*10^-8</f>
+        <v>1.7240000000000001E-8</v>
+      </c>
+      <c r="BE135" t="s">
+        <v>159</v>
+      </c>
+      <c r="BF135">
+        <v>1</v>
+      </c>
+      <c r="BG135">
+        <v>9.0999999999999998E-2</v>
+      </c>
+      <c r="BH135" s="23">
+        <f>BF135/BG135</f>
+        <v>10.989010989010989</v>
+      </c>
+      <c r="BI135" t="s">
+        <v>157</v>
+      </c>
+      <c r="BL135" s="1" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="136" spans="5:64" ht="15" thickBot="1">
       <c r="E136" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F136">
         <f>F132*F137*F140</f>
         <v>5.7189249421773602E-4</v>
       </c>
       <c r="J136" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="O136" t="s">
+        <v>135</v>
+      </c>
+      <c r="P136">
+        <f>(P132*P138)      *    ((Q115*P123 *     (Q117/Q118))/(Q114/1000))</f>
+        <v>630.89947163552404</v>
+      </c>
+      <c r="T136" t="s">
         <v>136</v>
       </c>
-      <c r="P136" t="e">
-        <f>P132*P138*P144</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="T136" t="s">
-        <v>137</v>
-      </c>
       <c r="U136" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="137" spans="5:42" x14ac:dyDescent="0.3">
+        <v>142</v>
+      </c>
+      <c r="AZ136" t="s">
+        <v>99</v>
+      </c>
+      <c r="BB136">
+        <f>2.43*10^-8</f>
+        <v>2.4300000000000003E-8</v>
+      </c>
+      <c r="BF136" s="9">
+        <f>BF134/BF135</f>
+        <v>0.7</v>
+      </c>
+      <c r="BG136" s="10">
+        <f>BG134/BG135</f>
+        <v>1.098901098901099</v>
+      </c>
+    </row>
+    <row r="137" spans="5:64">
       <c r="E137" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F137">
         <v>1</v>
       </c>
       <c r="O137" t="s">
+        <v>143</v>
+      </c>
+      <c r="P137">
+        <f>(P132*P138)      *    ((Q115*P123/     (Q117/Q118))/(Q114/1000))</f>
+        <v>39.431216977220252</v>
+      </c>
+      <c r="T137" t="s">
+        <v>145</v>
+      </c>
+      <c r="U137" t="s">
         <v>144</v>
       </c>
-      <c r="P137">
-        <f>P132*P138*((Q115*P123)/(Q114/1000))</f>
-        <v>157.72486790888101</v>
-      </c>
-      <c r="T137" t="s">
-        <v>146</v>
-      </c>
-      <c r="U137" t="s">
-        <v>145</v>
-      </c>
       <c r="AK137" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="AL137">
         <f>AM115*AL123/AP116</f>
         <v>3033.5564947856706</v>
       </c>
     </row>
-    <row r="138" spans="5:42" x14ac:dyDescent="0.3">
+    <row r="138" spans="5:64">
       <c r="O138" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="P138">
         <v>1000</v>
       </c>
       <c r="AK138" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="AL138">
         <f>AM115*AL123/(AP117*10^-2)</f>
         <v>99114.067501989965</v>
       </c>
       <c r="AP138" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="140" spans="5:42" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+      <c r="AZ138" t="s">
+        <v>95</v>
+      </c>
+      <c r="BA138">
+        <f>BA139*BA145*BA140*BA130</f>
+        <v>315.42589410241055</v>
+      </c>
+      <c r="BE138" t="s">
+        <v>128</v>
+      </c>
+      <c r="BH138" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="139" spans="5:64">
+      <c r="AZ139" t="s">
+        <v>96</v>
+      </c>
+      <c r="BA139">
+        <f>4*PI()*10^-7</f>
+        <v>1.2566370614359173E-6</v>
+      </c>
+    </row>
+    <row r="140" spans="5:64">
       <c r="E140" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F140">
         <f>G115*F123/J116</f>
         <v>455.09758685952926</v>
       </c>
       <c r="J140" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="141" spans="5:42" x14ac:dyDescent="0.3">
+        <v>130</v>
+      </c>
+      <c r="AZ140" t="s">
+        <v>112</v>
+      </c>
+      <c r="BA140">
+        <f>(BB116/(BB115/1000))</f>
+        <v>5000</v>
+      </c>
+      <c r="BE140" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="141" spans="5:64">
       <c r="E141" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F141">
         <f>G115*F123/(J117*10^-3)</f>
         <v>285946.24710886803</v>
       </c>
       <c r="J141" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="O141" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="P141">
         <f>((P137^2)*Z141)/(2*P138*P132)</f>
-        <v>0.31096417446092456</v>
+        <v>1.9435260903807785E-2</v>
       </c>
       <c r="T141" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="X141" t="s">
+        <v>147</v>
+      </c>
+      <c r="Y141" t="s">
         <v>148</v>
-      </c>
-      <c r="Y141" t="s">
-        <v>149</v>
       </c>
       <c r="Z141">
         <f>PI()*(Q127/2000)^2</f>
         <v>3.1415926535897931E-8</v>
       </c>
-    </row>
-    <row r="142" spans="5:42" x14ac:dyDescent="0.3">
+      <c r="AZ141" t="s">
+        <v>125</v>
+      </c>
+      <c r="BA141">
+        <f>BA139*BA145*BA152</f>
+        <v>477.9180213672887</v>
+      </c>
+      <c r="BE141" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="142" spans="5:64">
       <c r="E142" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F142">
         <f>G116*F124/(G114*10^-3)</f>
         <v>64699.188250217609</v>
       </c>
       <c r="J142" t="s">
+        <v>132</v>
+      </c>
+      <c r="AZ142" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="144" spans="5:42" x14ac:dyDescent="0.3">
+      <c r="BA142">
+        <f>BA139*BA145*(BB115*10^-2)</f>
+        <v>1.2566370614359175E-5</v>
+      </c>
+      <c r="BE142" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="143" spans="5:64">
+      <c r="AZ143" t="s">
+        <v>135</v>
+      </c>
+      <c r="BA143">
+        <f>BA139*BA145*BA151</f>
+        <v>0.47791802136728873</v>
+      </c>
+      <c r="BE143" t="s">
+        <v>136</v>
+      </c>
+      <c r="BF143" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="144" spans="5:64">
       <c r="O144" t="s">
-        <v>117</v>
-      </c>
-      <c r="P144" t="e">
-        <f>Q109*(Q113/Q114)*P123/T111</f>
-        <v>#VALUE!</v>
+        <v>116</v>
+      </c>
+      <c r="P144">
+        <f>Q115*(Q117/Q118)*P123/T116</f>
+        <v>12314.900106070776</v>
       </c>
       <c r="T144" t="s">
+        <v>130</v>
+      </c>
+      <c r="AZ144" t="s">
+        <v>143</v>
+      </c>
+      <c r="BA144">
+        <f>BA139*BA145*((BB116*BA130)/(BB115/1000))</f>
+        <v>315.42589410241055</v>
+      </c>
+      <c r="BE144" t="s">
+        <v>145</v>
+      </c>
+      <c r="BF144" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="145" spans="3:58">
+      <c r="O145" t="s">
+        <v>124</v>
+      </c>
+      <c r="P145">
+        <f>Q115*P123/(Q114*10^-3)</f>
+        <v>125513.46188107334</v>
+      </c>
+      <c r="T145" t="s">
+        <v>141</v>
+      </c>
+      <c r="AZ145" t="s">
+        <v>127</v>
+      </c>
+      <c r="BA145">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="146" spans="3:58">
+      <c r="O146" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="145" spans="3:20" x14ac:dyDescent="0.3">
-      <c r="O145" t="s">
-        <v>125</v>
-      </c>
-      <c r="P145" t="e">
-        <f>Q109*P123/(T112*10^-3)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="T145" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="146" spans="3:20" x14ac:dyDescent="0.3">
-      <c r="O146" t="s">
+      <c r="P146">
+        <f>Q115*P123/(Q114*10^-3)</f>
+        <v>125513.46188107334</v>
+      </c>
+      <c r="T146" t="s">
         <v>132</v>
       </c>
-      <c r="P146" t="e">
-        <f>Q111*P124/(Q108*10^-3)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="T146" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="148" spans="3:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="147" spans="3:58">
+      <c r="AZ147" t="s">
+        <v>147</v>
+      </c>
+      <c r="BA147">
+        <f>PI()*(BB134/2000)^2</f>
+        <v>2.5446900494077322E-6</v>
+      </c>
+      <c r="BE147" t="s">
+        <v>148</v>
+      </c>
+      <c r="BF147" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="148" spans="3:58" ht="15" thickBot="1">
       <c r="C148" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="149" spans="3:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>152</v>
+      </c>
+      <c r="V148" t="s">
+        <v>153</v>
+      </c>
+      <c r="AZ148" t="s">
+        <v>146</v>
+      </c>
+      <c r="BA148">
+        <f>((BA144^2)*BA147)/(2*BA145*BA139)</f>
+        <v>1007.3716335368391</v>
+      </c>
+      <c r="BE148" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="149" spans="3:58" ht="15" thickBot="1">
       <c r="D149" t="s">
         <v>79</v>
       </c>
       <c r="E149" s="11" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="150" spans="3:20" x14ac:dyDescent="0.3">
+      <c r="W149" t="s">
+        <v>79</v>
+      </c>
+      <c r="X149" s="11" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="150" spans="3:58">
       <c r="G150" s="14" t="s">
         <v>80</v>
       </c>
@@ -2499,8 +3059,20 @@
       <c r="J150" s="12" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="151" spans="3:20" x14ac:dyDescent="0.3">
+      <c r="Z150" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="AA150" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="AB150" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC150" s="12" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="151" spans="3:58">
       <c r="E151" s="15" t="s">
         <v>84</v>
       </c>
@@ -2518,52 +3090,137 @@
         <f>(H151*2)+(I151*2)</f>
         <v>12</v>
       </c>
-    </row>
-    <row r="152" spans="3:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="X151" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="Y151" s="15"/>
+      <c r="Z151" s="12">
+        <v>10</v>
+      </c>
+      <c r="AA151" s="13">
+        <v>10</v>
+      </c>
+      <c r="AB151" s="12">
+        <f>30+(4/(AA151))*2</f>
+        <v>30.8</v>
+      </c>
+      <c r="AC151" s="12">
+        <f>(AA151*2)+(AB151*2)</f>
+        <v>81.599999999999994</v>
+      </c>
+      <c r="AE151">
+        <f>(((AA151*2)+(AB151*2))*Z154)   +( Z154*  (2*(AA151+Z170)+(2*(AB151+Z170))))   +   (Z154*      (2*(AA151+Z170*2)) +(2*(AB151+Z170*2)))</f>
+        <v>2761.5428571428574</v>
+      </c>
+      <c r="AZ151" t="s">
+        <v>116</v>
+      </c>
+      <c r="BA151">
+        <f>BB116*(BB120/BB121)*BA130/BE117</f>
+        <v>3803.1507746651023</v>
+      </c>
+      <c r="BE151" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="152" spans="3:58" ht="15" thickBot="1">
       <c r="E152" s="15" t="s">
         <v>107</v>
       </c>
       <c r="F152" s="15"/>
       <c r="G152" s="12">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="153" spans="3:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>28</v>
+      </c>
+      <c r="X152" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="Y152" s="15"/>
+      <c r="Z152" s="12">
+        <v>30</v>
+      </c>
+      <c r="AZ152" t="s">
+        <v>124</v>
+      </c>
+      <c r="BA152">
+        <f>BB116*BA130/(BE117*10^-3)</f>
+        <v>3803150.7746651024</v>
+      </c>
+      <c r="BE152" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="153" spans="3:58" ht="15" thickBot="1">
       <c r="E153" s="15" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F153" s="15"/>
       <c r="G153" s="12">
         <f>J151*G152*(G156/G157)</f>
-        <v>1200</v>
+        <v>336</v>
       </c>
       <c r="I153" s="9" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="J153" s="10">
         <f>G153/1000</f>
-        <v>1.2</v>
-      </c>
-    </row>
-    <row r="154" spans="3:20" x14ac:dyDescent="0.3">
+        <v>0.33600000000000002</v>
+      </c>
+      <c r="X153" s="15" t="s">
+        <v>137</v>
+      </c>
+      <c r="Y153" s="15"/>
+      <c r="Z153" s="12">
+        <f>AC151*Z152*(Z156/Z157)</f>
+        <v>2448</v>
+      </c>
+      <c r="AB153" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="AC153" s="10">
+        <f>Z153/1000</f>
+        <v>2.448</v>
+      </c>
+      <c r="AE153">
+        <f>AE151/1000</f>
+        <v>2.7615428571428575</v>
+      </c>
+      <c r="AZ153" t="s">
+        <v>131</v>
+      </c>
+      <c r="BA153">
+        <f>(BB116)*BA130/(BB115*10^-3)</f>
+        <v>2510079.5112789674</v>
+      </c>
+      <c r="BE153" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="154" spans="3:58">
       <c r="D154" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G154">
         <f>(2*PI()*J155*G152) *(G156/G157)</f>
-        <v>6283.1853071795858</v>
+        <v>1759.2918860102841</v>
       </c>
       <c r="I154" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="J154">
         <f>G154/1000</f>
-        <v>6.2831853071795862</v>
-      </c>
-    </row>
-    <row r="155" spans="3:20" x14ac:dyDescent="0.3">
+        <v>1.7592918860102842</v>
+      </c>
+      <c r="X154" s="25" t="s">
+        <v>169</v>
+      </c>
+      <c r="Z154">
+        <f>Z151/Z170</f>
+        <v>14.285714285714286</v>
+      </c>
+    </row>
+    <row r="155" spans="3:58">
       <c r="I155" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="J155">
         <v>10</v>
@@ -2573,7 +3230,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="156" spans="3:20" x14ac:dyDescent="0.3">
+    <row r="156" spans="3:58" ht="15" thickBot="1">
       <c r="E156" s="15" t="s">
         <v>106</v>
       </c>
@@ -2581,8 +3238,21 @@
       <c r="G156">
         <v>3</v>
       </c>
-    </row>
-    <row r="157" spans="3:20" x14ac:dyDescent="0.3">
+      <c r="X156" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="Y156" s="15"/>
+      <c r="Z156">
+        <v>3</v>
+      </c>
+      <c r="AD156" t="s">
+        <v>161</v>
+      </c>
+      <c r="AG156">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="157" spans="3:58" ht="15" thickBot="1">
       <c r="E157" s="15" t="s">
         <v>105</v>
       </c>
@@ -2590,8 +3260,24 @@
       <c r="G157">
         <v>3</v>
       </c>
-    </row>
-    <row r="162" spans="5:13" x14ac:dyDescent="0.3">
+      <c r="X157" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="Y157" s="15"/>
+      <c r="Z157">
+        <v>3</v>
+      </c>
+      <c r="AD157" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="AE157" s="24"/>
+      <c r="AF157" s="24"/>
+      <c r="AG157" s="10">
+        <f>Y166/AG156</f>
+        <v>54.712749087955167</v>
+      </c>
+    </row>
+    <row r="162" spans="5:36">
       <c r="E162" s="16" t="s">
         <v>100</v>
       </c>
@@ -2601,8 +3287,17 @@
       <c r="G162" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="163" spans="5:13" x14ac:dyDescent="0.3">
+      <c r="X162" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="Y162">
+        <v>2</v>
+      </c>
+      <c r="Z162" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="163" spans="5:36">
       <c r="E163" s="12" t="s">
         <v>94</v>
       </c>
@@ -2612,8 +3307,17 @@
       <c r="G163" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="164" spans="5:13" x14ac:dyDescent="0.3">
+      <c r="X163" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="Y163">
+        <v>12</v>
+      </c>
+      <c r="Z163" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="164" spans="5:36">
       <c r="E164" s="12" t="s">
         <v>35</v>
       </c>
@@ -2623,8 +3327,17 @@
       <c r="G164" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="165" spans="5:13" x14ac:dyDescent="0.3">
+      <c r="X164" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="Y164" s="17">
+        <v>0</v>
+      </c>
+      <c r="Z164" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="165" spans="5:36">
       <c r="E165" s="12" t="s">
         <v>93</v>
       </c>
@@ -2635,56 +3348,126 @@
       <c r="G165" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="166" spans="5:13" x14ac:dyDescent="0.3">
+      <c r="X165" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="Y165">
+        <f>Y163-Y164</f>
+        <v>12</v>
+      </c>
+      <c r="Z165" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="166" spans="5:36">
       <c r="E166" s="12" t="s">
         <v>89</v>
       </c>
       <c r="F166">
         <f>F165/F168</f>
-        <v>111.61400813942856</v>
+        <v>398.62145764081623</v>
       </c>
       <c r="G166" t="s">
         <v>97</v>
       </c>
       <c r="J166" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="167" spans="5:13" x14ac:dyDescent="0.3">
+        <v>114</v>
+      </c>
+      <c r="X166" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="Y166">
+        <f>Y165/Y168</f>
+        <v>54.712749087955167</v>
+      </c>
+      <c r="Z166" t="s">
+        <v>97</v>
+      </c>
+      <c r="AC166" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="167" spans="5:36">
       <c r="E167" s="12" t="s">
         <v>90</v>
       </c>
       <c r="F167">
         <f>((G171)    *  (J153)      ) /(PI() * ((G170/2) * (1/1000))^2    )</f>
-        <v>5.3756693268328666E-2</v>
+        <v>1.5051874115132027E-2</v>
       </c>
       <c r="G167" s="18"/>
       <c r="J167" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="168" spans="5:13" x14ac:dyDescent="0.3">
+        <v>118</v>
+      </c>
+      <c r="X167" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="Y167">
+        <f>((Z171)    *  (AC153)      ) /(PI() * ((Z170/2) * (1/1000))^2    )</f>
+        <v>0.1096636542673905</v>
+      </c>
+      <c r="Z167" s="18"/>
+      <c r="AC167" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="168" spans="5:36">
       <c r="E168" s="19" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F168">
         <f>F167*F162</f>
-        <v>0.10751338653665733</v>
+        <v>3.0103748230264054E-2</v>
       </c>
       <c r="J168" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="170" spans="5:13" x14ac:dyDescent="0.3">
+        <v>115</v>
+      </c>
+      <c r="X168" s="19" t="s">
+        <v>110</v>
+      </c>
+      <c r="Y168">
+        <f>Y167*Y162</f>
+        <v>0.219327308534781</v>
+      </c>
+      <c r="AC168" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="169" spans="5:36" ht="15" thickBot="1"/>
+    <row r="170" spans="5:36">
       <c r="E170" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G170">
         <v>0.7</v>
       </c>
-    </row>
-    <row r="171" spans="5:13" x14ac:dyDescent="0.3">
+      <c r="X170" t="s">
+        <v>111</v>
+      </c>
+      <c r="Z170">
+        <v>0.7</v>
+      </c>
+      <c r="AC170" t="s">
+        <v>158</v>
+      </c>
+      <c r="AD170">
+        <v>0.7</v>
+      </c>
+      <c r="AE170">
+        <v>0.1</v>
+      </c>
+      <c r="AF170" s="22">
+        <f>AD170/AE170</f>
+        <v>6.9999999999999991</v>
+      </c>
+      <c r="AG170" t="s">
+        <v>155</v>
+      </c>
+      <c r="AJ170" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="171" spans="5:36" ht="15" thickBot="1">
       <c r="E171" t="s">
         <v>98</v>
       </c>
@@ -2692,8 +3475,34 @@
         <f>1.724*10^-8</f>
         <v>1.7240000000000001E-8</v>
       </c>
-    </row>
-    <row r="172" spans="5:13" x14ac:dyDescent="0.3">
+      <c r="X171" t="s">
+        <v>98</v>
+      </c>
+      <c r="Z171">
+        <f>1.724*10^-8</f>
+        <v>1.7240000000000001E-8</v>
+      </c>
+      <c r="AC171" t="s">
+        <v>159</v>
+      </c>
+      <c r="AD171">
+        <v>1</v>
+      </c>
+      <c r="AE171">
+        <v>9.0999999999999998E-2</v>
+      </c>
+      <c r="AF171" s="23">
+        <f>AD171/AE171</f>
+        <v>10.989010989010989</v>
+      </c>
+      <c r="AG171" t="s">
+        <v>157</v>
+      </c>
+      <c r="AJ171" s="1" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="172" spans="5:36" ht="15" thickBot="1">
       <c r="E172" t="s">
         <v>99</v>
       </c>
@@ -2701,23 +3510,51 @@
         <f>2.43*10^-8</f>
         <v>2.4300000000000003E-8</v>
       </c>
-    </row>
-    <row r="174" spans="5:13" x14ac:dyDescent="0.3">
+      <c r="X172" t="s">
+        <v>99</v>
+      </c>
+      <c r="Z172">
+        <f>2.43*10^-8</f>
+        <v>2.4300000000000003E-8</v>
+      </c>
+      <c r="AD172" s="9">
+        <f>AD170/AD171</f>
+        <v>0.7</v>
+      </c>
+      <c r="AE172" s="10">
+        <f>AE170/AE171</f>
+        <v>1.098901098901099</v>
+      </c>
+    </row>
+    <row r="174" spans="5:36">
       <c r="E174" t="s">
         <v>95</v>
       </c>
       <c r="F174">
         <f>F175*F181*F176*F166</f>
-        <v>140.25829920341607</v>
+        <v>140.25829920341604</v>
       </c>
       <c r="J174" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="M174" s="1" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="175" spans="5:13" x14ac:dyDescent="0.3">
+        <v>117</v>
+      </c>
+      <c r="X174" t="s">
+        <v>95</v>
+      </c>
+      <c r="Y174">
+        <f>Y175*Y181*Y176*Y166</f>
+        <v>20.626220471090594</v>
+      </c>
+      <c r="AC174" t="s">
+        <v>128</v>
+      </c>
+      <c r="AF174" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="175" spans="5:36">
       <c r="E175" t="s">
         <v>96</v>
       </c>
@@ -2725,142 +3562,687 @@
         <f>4*PI()*10^-7</f>
         <v>1.2566370614359173E-6</v>
       </c>
-    </row>
-    <row r="176" spans="5:13" x14ac:dyDescent="0.3">
+      <c r="X175" t="s">
+        <v>96</v>
+      </c>
+      <c r="Y175">
+        <f>4*PI()*10^-7</f>
+        <v>1.2566370614359173E-6</v>
+      </c>
+    </row>
+    <row r="176" spans="5:36">
       <c r="E176" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F176">
         <f>(G152/(G151/1000))</f>
-        <v>10000</v>
+        <v>2800</v>
       </c>
       <c r="J176" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="177" spans="5:11" x14ac:dyDescent="0.3">
+        <v>119</v>
+      </c>
+      <c r="X176" t="s">
+        <v>112</v>
+      </c>
+      <c r="Y176">
+        <f>(Z152/(Z151/1000))</f>
+        <v>3000</v>
+      </c>
+      <c r="AC176" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="177" spans="5:30">
       <c r="E177" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F177">
         <f>F175*F181*F188</f>
-        <v>140.25829920341607</v>
+        <v>140.25829920341604</v>
       </c>
       <c r="J177" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="178" spans="5:11" x14ac:dyDescent="0.3">
+        <v>126</v>
+      </c>
+      <c r="X177" t="s">
+        <v>125</v>
+      </c>
+      <c r="Y177">
+        <f>Y175*Y181*Y188</f>
+        <v>84.257436564912553</v>
+      </c>
+      <c r="AC177" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="178" spans="5:30">
       <c r="E178" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F178">
         <f>F175*F181*(G151*10^-2)</f>
         <v>1.2566370614359175E-5</v>
       </c>
       <c r="J178" t="s">
+        <v>134</v>
+      </c>
+      <c r="X178" t="s">
+        <v>133</v>
+      </c>
+      <c r="Y178">
+        <f>Y175*Y181*(Z151*10^-2)</f>
+        <v>1.2566370614359175E-5</v>
+      </c>
+      <c r="AC178" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="179" spans="5:30">
+      <c r="E179" t="s">
         <v>135</v>
-      </c>
-    </row>
-    <row r="179" spans="5:11" x14ac:dyDescent="0.3">
-      <c r="E179" t="s">
-        <v>136</v>
       </c>
       <c r="F179">
         <f>F175*F181*F187</f>
-        <v>0.22322801627885716</v>
+        <v>0.7972429152816326</v>
       </c>
       <c r="J179" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="K179" t="s">
+        <v>142</v>
+      </c>
+      <c r="X179" t="s">
+        <v>135</v>
+      </c>
+      <c r="Y179">
+        <f>Y175*Y181*Y187</f>
+        <v>8.4257436564912566E-2</v>
+      </c>
+      <c r="AC179" t="s">
+        <v>136</v>
+      </c>
+      <c r="AD179" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="180" spans="5:30">
+      <c r="E180" t="s">
         <v>143</v>
-      </c>
-    </row>
-    <row r="180" spans="5:11" x14ac:dyDescent="0.3">
-      <c r="E180" t="s">
-        <v>144</v>
       </c>
       <c r="F180">
         <f>F175*F181*((G152*F166)/(G151/1000))</f>
-        <v>140.25829920341607</v>
+        <v>140.25829920341604</v>
       </c>
       <c r="J180" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="K180" t="s">
+        <v>144</v>
+      </c>
+      <c r="X180" t="s">
+        <v>143</v>
+      </c>
+      <c r="Y180">
+        <f>Y175*Y181*((Z152*Y166)/(Z151/1000))</f>
+        <v>20.626220471090594</v>
+      </c>
+      <c r="AC180" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="181" spans="5:11" x14ac:dyDescent="0.3">
+      <c r="AD180" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="181" spans="5:30">
       <c r="E181" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F181">
         <v>100</v>
       </c>
-    </row>
-    <row r="183" spans="5:11" x14ac:dyDescent="0.3">
+      <c r="X181" t="s">
+        <v>127</v>
+      </c>
+      <c r="Y181">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="183" spans="5:30">
       <c r="E183" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F183">
         <f>PI()*(G170/2000)^2</f>
         <v>3.8484510006474966E-7</v>
       </c>
       <c r="J183" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="K183" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="184" spans="5:11" x14ac:dyDescent="0.3">
+        <v>150</v>
+      </c>
+      <c r="X183" t="s">
+        <v>147</v>
+      </c>
+      <c r="Y183">
+        <f>PI()*(Z170/2000)^2</f>
+        <v>3.8484510006474966E-7</v>
+      </c>
+      <c r="AC183" t="s">
+        <v>148</v>
+      </c>
+      <c r="AD183" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="184" spans="5:30">
       <c r="E184" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F184">
         <f>((F180^2)*F183)/(2*F181*F175)</f>
-        <v>30.123347946134817</v>
+        <v>30.123347946134807</v>
       </c>
       <c r="J184" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="187" spans="5:11" x14ac:dyDescent="0.3">
+        <v>149</v>
+      </c>
+      <c r="X184" t="s">
+        <v>146</v>
+      </c>
+      <c r="Y184">
+        <f>((Y180^2)*Y183)/(2*Y181*Y175)</f>
+        <v>0.65145648672436862</v>
+      </c>
+      <c r="AC184" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="187" spans="5:30">
       <c r="E187" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F187">
         <f>G152*(G156/G157)*F166/J154</f>
-        <v>1776.3921113689098</v>
+        <v>6344.2575406032483</v>
       </c>
       <c r="J187" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="188" spans="5:11" x14ac:dyDescent="0.3">
+        <v>130</v>
+      </c>
+      <c r="X187" t="s">
+        <v>116</v>
+      </c>
+      <c r="Y187">
+        <f>Z152*(Z156/Z157)*Y166/AC153</f>
+        <v>670.49937607788195</v>
+      </c>
+      <c r="AC187" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="188" spans="5:30">
       <c r="E188" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F188">
         <f>G152*F166/(J155*10^-3)</f>
-        <v>1116140.0813942857</v>
+        <v>1116140.0813942854</v>
       </c>
       <c r="J188" t="s">
+        <v>141</v>
+      </c>
+      <c r="X188" t="s">
+        <v>124</v>
+      </c>
+      <c r="Y188">
+        <f>Z152*Y166/(AC153*10^-3)</f>
+        <v>670499.3760778819</v>
+      </c>
+      <c r="AC188" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="189" spans="5:30">
+      <c r="E189" t="s">
+        <v>131</v>
+      </c>
+      <c r="F189">
+        <f>(G152)*F166/(G151*10^-3)</f>
+        <v>1116140.0813942854</v>
+      </c>
+      <c r="J189" t="s">
+        <v>132</v>
+      </c>
+      <c r="X189" t="s">
+        <v>131</v>
+      </c>
+      <c r="Y189">
+        <f>(Z152)*Y166/(Z151*10^-3)</f>
+        <v>164138.24726386549</v>
+      </c>
+      <c r="AC189" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="196" spans="3:11" ht="15" thickBot="1">
+      <c r="C196" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="197" spans="3:11" ht="15" thickBot="1">
+      <c r="D197" t="s">
+        <v>79</v>
+      </c>
+      <c r="E197" s="11" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="198" spans="3:11">
+      <c r="G198" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="H198" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="I198" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="J198" s="12" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="199" spans="3:11">
+      <c r="E199" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="F199" s="15"/>
+      <c r="G199" s="12">
+        <v>10</v>
+      </c>
+      <c r="H199" s="13">
+        <v>3</v>
+      </c>
+      <c r="I199" s="12">
+        <v>3</v>
+      </c>
+      <c r="J199" s="12">
+        <f>(H199*2)+(I199*2)</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="200" spans="3:11" ht="15" thickBot="1">
+      <c r="E200" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="F200" s="15"/>
+      <c r="G200" s="12">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="201" spans="3:11" ht="15" thickBot="1">
+      <c r="E201" s="15" t="s">
+        <v>137</v>
+      </c>
+      <c r="F201" s="15"/>
+      <c r="G201" s="12">
+        <f>J199*G200*(G204/G205)</f>
+        <v>216</v>
+      </c>
+      <c r="I201" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="J201" s="10">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="202" spans="3:11">
+      <c r="D202" t="s">
+        <v>138</v>
+      </c>
+      <c r="G202">
+        <f>(2*PI()*J203*G200) *(G204/G205)</f>
+        <v>1130.9733552923256</v>
+      </c>
+      <c r="I202" t="s">
+        <v>139</v>
+      </c>
+      <c r="J202">
+        <f>G202/1000</f>
+        <v>1.1309733552923256</v>
+      </c>
+    </row>
+    <row r="203" spans="3:11">
+      <c r="I203" t="s">
+        <v>129</v>
+      </c>
+      <c r="J203">
+        <v>10</v>
+      </c>
+      <c r="K203">
+        <f>K199/(2*PI())</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="204" spans="3:11">
+      <c r="E204" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="F204" s="15"/>
+      <c r="G204">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="205" spans="3:11">
+      <c r="E205" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="F205" s="15"/>
+      <c r="G205">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="210" spans="5:13">
+      <c r="E210" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="F210">
+        <v>2</v>
+      </c>
+      <c r="G210" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="211" spans="5:13">
+      <c r="E211" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="F211">
+        <v>12</v>
+      </c>
+      <c r="G211" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="212" spans="5:13">
+      <c r="E212" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="F212" s="17">
+        <v>0</v>
+      </c>
+      <c r="G212" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="213" spans="5:13">
+      <c r="E213" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="F213">
+        <f>F211-F212</f>
+        <v>12</v>
+      </c>
+      <c r="G213" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="214" spans="5:13">
+      <c r="E214" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="F214">
+        <f>F213/F216</f>
+        <v>595.33545239430691</v>
+      </c>
+      <c r="G214" t="s">
+        <v>97</v>
+      </c>
+      <c r="J214" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="215" spans="5:13">
+      <c r="E215" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="F215">
+        <f>((G219)    *  (J201)      ) /(PI() * ((G218/2) * (1/1000))^2    )</f>
+        <v>1.007835158458871E-2</v>
+      </c>
+      <c r="G215" s="18"/>
+      <c r="J215" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="216" spans="5:13">
+      <c r="E216" s="19" t="s">
+        <v>110</v>
+      </c>
+      <c r="F216">
+        <f>F215*F210</f>
+        <v>2.015670316917742E-2</v>
+      </c>
+      <c r="J216" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="218" spans="5:13">
+      <c r="E218" t="s">
+        <v>111</v>
+      </c>
+      <c r="G218">
+        <v>1.32</v>
+      </c>
+    </row>
+    <row r="219" spans="5:13">
+      <c r="E219" t="s">
+        <v>98</v>
+      </c>
+      <c r="G219">
+        <f>1.724*10^-8</f>
+        <v>1.7240000000000001E-8</v>
+      </c>
+    </row>
+    <row r="220" spans="5:13">
+      <c r="E220" t="s">
+        <v>99</v>
+      </c>
+      <c r="G220">
+        <f>2.43*10^-8</f>
+        <v>2.4300000000000003E-8</v>
+      </c>
+    </row>
+    <row r="222" spans="5:13">
+      <c r="E222" t="s">
+        <v>95</v>
+      </c>
+      <c r="F222">
+        <f>F223*F229*F224*F214</f>
+        <v>3.7406029673270214E-3</v>
+      </c>
+      <c r="J222" t="s">
+        <v>128</v>
+      </c>
+      <c r="M222" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="223" spans="5:13">
+      <c r="E223" t="s">
+        <v>96</v>
+      </c>
+      <c r="F223">
+        <f>4*PI()*10^-7</f>
+        <v>1.2566370614359173E-6</v>
+      </c>
+    </row>
+    <row r="224" spans="5:13">
+      <c r="E224" t="s">
+        <v>112</v>
+      </c>
+      <c r="F224">
+        <v>5</v>
+      </c>
+      <c r="J224" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="225" spans="5:11">
+      <c r="E225" t="s">
+        <v>125</v>
+      </c>
+      <c r="F225">
+        <f>F223*F229*F236</f>
+        <v>1.3466170682377279</v>
+      </c>
+      <c r="J225" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="226" spans="5:11">
+      <c r="E226" t="s">
+        <v>133</v>
+      </c>
+      <c r="F226">
+        <f>F223*F229*(G199*10^-2)</f>
+        <v>1.2566370614359172E-7</v>
+      </c>
+      <c r="J226" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="227" spans="5:11">
+      <c r="E227" t="s">
+        <v>135</v>
+      </c>
+      <c r="F227">
+        <f>F223*F229*F235</f>
+        <v>1.1906709047886139E-2</v>
+      </c>
+      <c r="J227" t="s">
+        <v>136</v>
+      </c>
+      <c r="K227" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="189" spans="5:11" x14ac:dyDescent="0.3">
-      <c r="E189" t="s">
+    <row r="228" spans="5:11">
+      <c r="E228" t="s">
+        <v>143</v>
+      </c>
+      <c r="F228">
+        <f>F223*F229*((G200*F214)/(G199/1000))</f>
+        <v>1.3466170682377279</v>
+      </c>
+      <c r="J228" t="s">
+        <v>145</v>
+      </c>
+      <c r="K228" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="229" spans="5:11">
+      <c r="E229" t="s">
+        <v>127</v>
+      </c>
+      <c r="F229">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="231" spans="5:11">
+      <c r="E231" t="s">
+        <v>147</v>
+      </c>
+      <c r="F231">
+        <f>PI()*(G218/2000)^2</f>
+        <v>1.3684777599037139E-6</v>
+      </c>
+      <c r="J231" t="s">
+        <v>148</v>
+      </c>
+      <c r="K231" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="232" spans="5:11">
+      <c r="E232" t="s">
+        <v>146</v>
+      </c>
+      <c r="F232">
+        <f>((F228^2)*F231)/(2*F229*F223)</f>
+        <v>0.98738406425146485</v>
+      </c>
+      <c r="J232" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="235" spans="5:11">
+      <c r="E235" t="s">
+        <v>116</v>
+      </c>
+      <c r="F235">
+        <f>G200*(G204/G205)*F214/J202</f>
+        <v>9475.0580046403684</v>
+      </c>
+      <c r="J235" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="236" spans="5:11">
+      <c r="E236" t="s">
+        <v>124</v>
+      </c>
+      <c r="F236">
+        <f>G200*F214/(J203*10^-3)</f>
+        <v>1071603.8143097525</v>
+      </c>
+      <c r="J236" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="237" spans="5:11">
+      <c r="E237" t="s">
+        <v>131</v>
+      </c>
+      <c r="F237">
+        <f>G202*F214/(G199*10^-3)</f>
+        <v>67330853.411886379</v>
+      </c>
+      <c r="J237" t="s">
         <v>132</v>
       </c>
-      <c r="F189">
-        <f>G154*F167/(G151*10^-3)</f>
-        <v>33776.326530612241</v>
-      </c>
-      <c r="J189" t="s">
-        <v>133</v>
+    </row>
+    <row r="248" spans="3:3">
+      <c r="C248" s="1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="249" spans="3:3">
+      <c r="C249" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="250" spans="3:3">
+      <c r="C250" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="253" spans="3:3">
+      <c r="C253" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="254" spans="3:3" ht="16.2">
+      <c r="C254" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="258" spans="3:3">
+      <c r="C258" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="259" spans="3:3">
+      <c r="C259" t="s">
+        <v>168</v>
       </c>
     </row>
   </sheetData>
@@ -2888,6 +4270,17 @@
     <hyperlink ref="M174" r:id="rId5" xr:uid="{79751D78-4AEC-44DE-AC1E-BA8958ECC5B8}"/>
     <hyperlink ref="D98" r:id="rId6" xr:uid="{B7D8395C-6009-4E53-8ACA-509F289CCAF3}"/>
     <hyperlink ref="W131" r:id="rId7" xr:uid="{9A1BFDCD-A14D-44F9-B3A7-1B4DD4B5B216}"/>
+    <hyperlink ref="M222" r:id="rId8" xr:uid="{C536941B-66A7-404F-9D95-B6AFA64846EF}"/>
+    <hyperlink ref="AF174" r:id="rId9" xr:uid="{3C76D7FA-957A-4187-B2E1-EB69B73B03E9}"/>
+    <hyperlink ref="AJ170" r:id="rId10" xr:uid="{F1F26B2B-D79F-4806-A039-EA4CD8A46268}"/>
+    <hyperlink ref="AJ171" r:id="rId11" xr:uid="{B293B513-DBD9-4A0D-B1AE-D724A5084D91}"/>
+    <hyperlink ref="C248" r:id="rId12" xr:uid="{34C3619C-5BDB-4DD3-ABB1-AB540962BC3B}"/>
+    <hyperlink ref="C253" r:id="rId13" xr:uid="{28DDD3BE-8F1C-4618-B1F7-71E2A155EC29}"/>
+    <hyperlink ref="C258" r:id="rId14" xr:uid="{09DBD9BD-FCC2-4D91-BFC9-A835238C46D9}"/>
+    <hyperlink ref="BH138" r:id="rId15" xr:uid="{E997DB2D-53B9-4758-8A48-DA0245BFB158}"/>
+    <hyperlink ref="BL134" r:id="rId16" xr:uid="{C19962B2-E084-4855-AA70-DF3367C31B2C}"/>
+    <hyperlink ref="BL135" r:id="rId17" xr:uid="{2151C8A9-E276-49A9-B3F5-BF2B8ECE7620}"/>
+    <hyperlink ref="AX111" r:id="rId18" xr:uid="{79B7784E-B59D-40D1-BC55-2DEF7EF5CCAC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
revision of every model
purpose:
	- fixing errors in model for slicer program
</commit_message>
<xml_diff>
--- a/Documentations/sequence.xlsx
+++ b/Documentations/sequence.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\school\2ndyr\1stsem\emag\generotr\Documentations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B12B96E-EEE0-43BF-8232-FCCCBFC9DF18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C585F67E-20D5-4447-BA13-BA91E6B0BEF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A0CABE93-1CAF-4178-A500-DBCC18B4841B}"/>
   </bookViews>
@@ -891,19 +891,19 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1221,8 +1221,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F298B35-6B67-4A34-9984-D13A8F00E275}">
   <dimension ref="C4:BL259"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A96" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="P106" sqref="P106"/>
+    <sheetView tabSelected="1" topLeftCell="P147" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Z153" sqref="Z153"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1753,7 +1753,7 @@
       </c>
     </row>
     <row r="98" spans="3:50">
-      <c r="C98" s="20" t="s">
+      <c r="C98" s="25" t="s">
         <v>121</v>
       </c>
       <c r="D98" s="1" t="s">
@@ -1761,7 +1761,7 @@
       </c>
     </row>
     <row r="99" spans="3:50">
-      <c r="C99" s="20"/>
+      <c r="C99" s="25"/>
     </row>
     <row r="102" spans="3:50">
       <c r="C102" t="s">
@@ -1787,10 +1787,10 @@
       </c>
     </row>
     <row r="106" spans="3:50" ht="28.8">
-      <c r="C106" s="26" t="s">
+      <c r="C106" s="24" t="s">
         <v>172</v>
       </c>
-      <c r="F106" s="26">
+      <c r="F106" s="24">
         <v>21.5</v>
       </c>
     </row>
@@ -1887,10 +1887,10 @@
       </c>
     </row>
     <row r="114" spans="5:61">
-      <c r="E114" s="21" t="s">
+      <c r="E114" s="26" t="s">
         <v>84</v>
       </c>
-      <c r="F114" s="21"/>
+      <c r="F114" s="26"/>
       <c r="G114" s="12">
         <v>18</v>
       </c>
@@ -1909,10 +1909,10 @@
         <f>(H114*2)+(I114*2)+(J114*4)</f>
         <v>66.283185307179593</v>
       </c>
-      <c r="O114" s="21" t="s">
+      <c r="O114" s="26" t="s">
         <v>84</v>
       </c>
-      <c r="P114" s="21"/>
+      <c r="P114" s="26"/>
       <c r="Q114" s="12">
         <v>5</v>
       </c>
@@ -1926,10 +1926,10 @@
         <f>(R114*2)+(S114*2)</f>
         <v>3.92</v>
       </c>
-      <c r="AK114" s="21" t="s">
+      <c r="AK114" s="26" t="s">
         <v>84</v>
       </c>
-      <c r="AL114" s="21"/>
+      <c r="AL114" s="26"/>
       <c r="AM114" s="12">
         <v>5</v>
       </c>
@@ -1957,24 +1957,24 @@
       </c>
     </row>
     <row r="115" spans="5:61" ht="15" thickBot="1">
-      <c r="E115" s="21" t="s">
+      <c r="E115" s="26" t="s">
         <v>85</v>
       </c>
-      <c r="F115" s="21"/>
+      <c r="F115" s="26"/>
       <c r="G115" s="12">
         <v>100</v>
       </c>
-      <c r="O115" s="21" t="s">
+      <c r="O115" s="26" t="s">
         <v>107</v>
       </c>
-      <c r="P115" s="21"/>
+      <c r="P115" s="26"/>
       <c r="Q115" s="12">
         <v>13</v>
       </c>
-      <c r="AK115" s="21" t="s">
+      <c r="AK115" s="26" t="s">
         <v>107</v>
       </c>
-      <c r="AL115" s="21"/>
+      <c r="AL115" s="26"/>
       <c r="AM115" s="12">
         <v>13</v>
       </c>
@@ -2001,10 +2001,10 @@
       </c>
     </row>
     <row r="116" spans="5:61" ht="15" thickBot="1">
-      <c r="E116" s="21" t="s">
+      <c r="E116" s="26" t="s">
         <v>88</v>
       </c>
-      <c r="F116" s="21"/>
+      <c r="F116" s="26"/>
       <c r="G116" s="12">
         <f>K114*G115</f>
         <v>6628.3185307179592</v>
@@ -2016,10 +2016,10 @@
         <f>G116/1000</f>
         <v>6.6283185307179595</v>
       </c>
-      <c r="O116" s="21" t="s">
+      <c r="O116" s="26" t="s">
         <v>88</v>
       </c>
-      <c r="P116" s="21"/>
+      <c r="P116" s="26"/>
       <c r="Q116" s="12">
         <f>T114*Q115*(Q117/Q118)</f>
         <v>203.84</v>
@@ -2031,10 +2031,10 @@
         <f>Q116/1000</f>
         <v>0.20383999999999999</v>
       </c>
-      <c r="AK116" s="21" t="s">
+      <c r="AK116" s="26" t="s">
         <v>88</v>
       </c>
-      <c r="AL116" s="21"/>
+      <c r="AL116" s="26"/>
       <c r="AM116" s="12">
         <f>AP114*AM115*(AM117/AM118)</f>
         <v>197.6</v>
@@ -2068,10 +2068,10 @@
         <f>K114/(2*PI())</f>
         <v>10.549296585513721</v>
       </c>
-      <c r="O117" s="21" t="s">
+      <c r="O117" s="26" t="s">
         <v>106</v>
       </c>
-      <c r="P117" s="21"/>
+      <c r="P117" s="26"/>
       <c r="Q117">
         <v>12</v>
       </c>
@@ -2082,10 +2082,10 @@
         <f>T114/(2*PI())</f>
         <v>0.62388737692022977</v>
       </c>
-      <c r="AK117" s="21" t="s">
+      <c r="AK117" s="26" t="s">
         <v>106</v>
       </c>
-      <c r="AL117" s="21"/>
+      <c r="AL117" s="26"/>
       <c r="AM117">
         <v>12</v>
       </c>
@@ -2123,21 +2123,21 @@
       <c r="G118">
         <v>3</v>
       </c>
-      <c r="O118" s="21" t="s">
+      <c r="O118" s="26" t="s">
         <v>105</v>
       </c>
-      <c r="P118" s="21"/>
+      <c r="P118" s="26"/>
       <c r="Q118">
         <v>3</v>
       </c>
-      <c r="AK118" s="21" t="s">
+      <c r="AK118" s="26" t="s">
         <v>105</v>
       </c>
-      <c r="AL118" s="21"/>
+      <c r="AL118" s="26"/>
       <c r="AM118">
         <v>3</v>
       </c>
-      <c r="AZ118" s="25" t="s">
+      <c r="AZ118" s="23" t="s">
         <v>169</v>
       </c>
       <c r="BB118">
@@ -2188,7 +2188,8 @@
         <v>94</v>
       </c>
       <c r="P120">
-        <v>11.82</v>
+        <f>11.5/10</f>
+        <v>1.1499999999999999</v>
       </c>
       <c r="V120" t="s">
         <v>161</v>
@@ -2233,7 +2234,7 @@
         <v>35</v>
       </c>
       <c r="P121">
-        <v>1.02</v>
+        <v>0.5</v>
       </c>
       <c r="Q121">
         <v>3.9</v>
@@ -2241,11 +2242,11 @@
       <c r="V121" s="9" t="s">
         <v>160</v>
       </c>
-      <c r="W121" s="24"/>
-      <c r="X121" s="24"/>
+      <c r="W121" s="22"/>
+      <c r="X121" s="22"/>
       <c r="Y121" s="10">
         <f>P123/Y120</f>
-        <v>530.48800456920264</v>
+        <v>31.927518793516821</v>
       </c>
       <c r="AK121" s="12" t="s">
         <v>35</v>
@@ -2266,8 +2267,8 @@
       <c r="BF121" s="9" t="s">
         <v>160</v>
       </c>
-      <c r="BG121" s="24"/>
-      <c r="BH121" s="24"/>
+      <c r="BG121" s="22"/>
+      <c r="BH121" s="22"/>
       <c r="BI121" s="10">
         <f>BA130/BI120</f>
         <v>67.83998679132344</v>
@@ -2289,7 +2290,7 @@
       </c>
       <c r="P122">
         <f>P120-P121</f>
-        <v>10.8</v>
+        <v>0.64999999999999991</v>
       </c>
       <c r="AK122" s="12" t="s">
         <v>93</v>
@@ -2318,7 +2319,7 @@
       </c>
       <c r="P123" s="17">
         <f>P122/(P125)</f>
-        <v>48.274408415797438</v>
+        <v>2.9054042102100306</v>
       </c>
       <c r="AK123" s="12" t="s">
         <v>89</v>
@@ -2529,7 +2530,7 @@
       </c>
       <c r="P131">
         <f>P132*P138*P133*P123</f>
-        <v>951.20228031202112</v>
+        <v>57.248285389149409</v>
       </c>
       <c r="T131" t="s">
         <v>128</v>
@@ -2640,7 +2641,7 @@
       </c>
       <c r="P134">
         <f>P132*P138*P145</f>
-        <v>157.72486790888101</v>
+        <v>9.4927003834048751</v>
       </c>
       <c r="T134" t="s">
         <v>126</v>
@@ -2670,7 +2671,7 @@
       <c r="BG134">
         <v>0.1</v>
       </c>
-      <c r="BH134" s="22">
+      <c r="BH134" s="20">
         <f>BF134/BG134</f>
         <v>6.9999999999999991</v>
       </c>
@@ -2697,7 +2698,7 @@
       </c>
       <c r="P135">
         <f>P132*P138*(P146*10^-3)</f>
-        <v>0.15772486790888102</v>
+        <v>9.4927003834048753E-3</v>
       </c>
       <c r="T135" t="s">
         <v>134</v>
@@ -2724,7 +2725,7 @@
       <c r="BG135">
         <v>9.0999999999999998E-2</v>
       </c>
-      <c r="BH135" s="23">
+      <c r="BH135" s="21">
         <f>BF135/BG135</f>
         <v>10.989010989010989</v>
       </c>
@@ -2751,7 +2752,7 @@
       </c>
       <c r="P136">
         <f>(P132*P138)      *    ((Q115*P123 *     (Q117/Q118))/(Q114/1000))</f>
-        <v>630.89947163552404</v>
+        <v>37.9708015336195</v>
       </c>
       <c r="T136" t="s">
         <v>136</v>
@@ -2787,7 +2788,7 @@
       </c>
       <c r="P137">
         <f>(P132*P138)      *    ((Q115*P123/     (Q117/Q118))/(Q114/1000))</f>
-        <v>39.431216977220252</v>
+        <v>2.3731750958512188</v>
       </c>
       <c r="T137" t="s">
         <v>145</v>
@@ -2881,7 +2882,7 @@
       </c>
       <c r="P141">
         <f>((P137^2)*Z141)/(2*P138*P132)</f>
-        <v>1.9435260903807785E-2</v>
+        <v>7.0399500444605516E-5</v>
       </c>
       <c r="T141" t="s">
         <v>149</v>
@@ -2950,7 +2951,7 @@
       </c>
       <c r="P144">
         <f>Q115*(Q117/Q118)*P123/T116</f>
-        <v>12314.900106070776</v>
+        <v>741.17454342092628</v>
       </c>
       <c r="T144" t="s">
         <v>130</v>
@@ -2975,7 +2976,7 @@
       </c>
       <c r="P145">
         <f>Q115*P123/(Q114*10^-3)</f>
-        <v>125513.46188107334</v>
+        <v>7554.05094654608</v>
       </c>
       <c r="T145" t="s">
         <v>141</v>
@@ -2993,7 +2994,7 @@
       </c>
       <c r="P146">
         <f>Q115*P123/(Q114*10^-3)</f>
-        <v>125513.46188107334</v>
+        <v>7554.05094654608</v>
       </c>
       <c r="T146" t="s">
         <v>132</v>
@@ -3136,7 +3137,7 @@
       </c>
       <c r="Y152" s="15"/>
       <c r="Z152" s="12">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="AZ152" t="s">
         <v>124</v>
@@ -3170,15 +3171,15 @@
       </c>
       <c r="Y153" s="15"/>
       <c r="Z153" s="12">
-        <f>AC151*Z152*(Z156/Z157)</f>
-        <v>2448</v>
+        <f>(AC151*Z152*(Z156/Z157))+300</f>
+        <v>4380</v>
       </c>
       <c r="AB153" s="9" t="s">
         <v>140</v>
       </c>
       <c r="AC153" s="10">
         <f>Z153/1000</f>
-        <v>2.448</v>
+        <v>4.38</v>
       </c>
       <c r="AE153">
         <f>AE151/1000</f>
@@ -3210,7 +3211,7 @@
         <f>G154/1000</f>
         <v>1.7592918860102842</v>
       </c>
-      <c r="X154" s="25" t="s">
+      <c r="X154" s="23" t="s">
         <v>169</v>
       </c>
       <c r="Z154">
@@ -3270,11 +3271,11 @@
       <c r="AD157" s="9" t="s">
         <v>160</v>
       </c>
-      <c r="AE157" s="24"/>
-      <c r="AF157" s="24"/>
+      <c r="AE157" s="22"/>
+      <c r="AF157" s="22"/>
       <c r="AG157" s="10">
         <f>Y166/AG156</f>
-        <v>54.712749087955167</v>
+        <v>1.9357555516410621</v>
       </c>
     </row>
     <row r="162" spans="5:36">
@@ -3311,7 +3312,8 @@
         <v>94</v>
       </c>
       <c r="Y163">
-        <v>12</v>
+        <f>11.5/10</f>
+        <v>1.1499999999999999</v>
       </c>
       <c r="Z163" t="s">
         <v>97</v>
@@ -3331,7 +3333,7 @@
         <v>35</v>
       </c>
       <c r="Y164" s="17">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="Z164" t="s">
         <v>97</v>
@@ -3353,7 +3355,7 @@
       </c>
       <c r="Y165">
         <f>Y163-Y164</f>
-        <v>12</v>
+        <v>1.0499999999999998</v>
       </c>
       <c r="Z165" t="s">
         <v>97</v>
@@ -3378,7 +3380,7 @@
       </c>
       <c r="Y166">
         <f>Y165/Y168</f>
-        <v>54.712749087955167</v>
+        <v>1.9357555516410621</v>
       </c>
       <c r="Z166" t="s">
         <v>97</v>
@@ -3404,7 +3406,7 @@
       </c>
       <c r="Y167">
         <f>((Z171)    *  (AC153)      ) /(PI() * ((Z170/2) * (1/1000))^2    )</f>
-        <v>0.1096636542673905</v>
+        <v>0.19621193042939963</v>
       </c>
       <c r="Z167" s="18"/>
       <c r="AC167" t="s">
@@ -3426,8 +3428,8 @@
         <v>110</v>
       </c>
       <c r="Y168">
-        <f>Y167*Y162</f>
-        <v>0.219327308534781</v>
+        <f>(Y167*Y162)+0.1+0.05</f>
+        <v>0.54242386085879934</v>
       </c>
       <c r="AC168" t="s">
         <v>115</v>
@@ -3456,7 +3458,7 @@
       <c r="AE170">
         <v>0.1</v>
       </c>
-      <c r="AF170" s="22">
+      <c r="AF170" s="20">
         <f>AD170/AE170</f>
         <v>6.9999999999999991</v>
       </c>
@@ -3491,7 +3493,7 @@
       <c r="AE171">
         <v>9.0999999999999998E-2</v>
       </c>
-      <c r="AF171" s="23">
+      <c r="AF171" s="21">
         <f>AD171/AE171</f>
         <v>10.989010989010989</v>
       </c>
@@ -3545,7 +3547,7 @@
       </c>
       <c r="Y174">
         <f>Y175*Y181*Y176*Y166</f>
-        <v>20.626220471090594</v>
+        <v>1.8244066260543654</v>
       </c>
       <c r="AC174" t="s">
         <v>128</v>
@@ -3586,7 +3588,7 @@
       </c>
       <c r="Y176">
         <f>(Z152/(Z151/1000))</f>
-        <v>3000</v>
+        <v>5000</v>
       </c>
       <c r="AC176" t="s">
         <v>119</v>
@@ -3608,7 +3610,7 @@
       </c>
       <c r="Y177">
         <f>Y175*Y181*Y188</f>
-        <v>84.257436564912553</v>
+        <v>4.1653119316309715</v>
       </c>
       <c r="AC177" t="s">
         <v>126</v>
@@ -3630,7 +3632,7 @@
       </c>
       <c r="Y178">
         <f>Y175*Y181*(Z151*10^-2)</f>
-        <v>1.2566370614359175E-5</v>
+        <v>1.8849555921538762E-5</v>
       </c>
       <c r="AC178" t="s">
         <v>134</v>
@@ -3655,7 +3657,7 @@
       </c>
       <c r="Y179">
         <f>Y175*Y181*Y187</f>
-        <v>8.4257436564912566E-2</v>
+        <v>4.1653119316309717E-3</v>
       </c>
       <c r="AC179" t="s">
         <v>136</v>
@@ -3683,7 +3685,7 @@
       </c>
       <c r="Y180">
         <f>Y175*Y181*((Z152*Y166)/(Z151/1000))</f>
-        <v>20.626220471090594</v>
+        <v>1.8244066260543657</v>
       </c>
       <c r="AC180" t="s">
         <v>145</v>
@@ -3703,7 +3705,7 @@
         <v>127</v>
       </c>
       <c r="Y181">
-        <v>100</v>
+        <v>150</v>
       </c>
     </row>
     <row r="183" spans="5:30">
@@ -3750,7 +3752,7 @@
       </c>
       <c r="Y184">
         <f>((Y180^2)*Y183)/(2*Y181*Y175)</f>
-        <v>0.65145648672436862</v>
+        <v>3.3978024442158881E-3</v>
       </c>
       <c r="AC184" t="s">
         <v>149</v>
@@ -3772,7 +3774,7 @@
       </c>
       <c r="Y187">
         <f>Z152*(Z156/Z157)*Y166/AC153</f>
-        <v>670.49937607788195</v>
+        <v>22.097666114623998</v>
       </c>
       <c r="AC187" t="s">
         <v>130</v>
@@ -3794,7 +3796,7 @@
       </c>
       <c r="Y188">
         <f>Z152*Y166/(AC153*10^-3)</f>
-        <v>670499.3760778819</v>
+        <v>22097.666114623997</v>
       </c>
       <c r="AC188" t="s">
         <v>141</v>
@@ -3816,7 +3818,7 @@
       </c>
       <c r="Y189">
         <f>(Z152)*Y166/(Z151*10^-3)</f>
-        <v>164138.24726386549</v>
+        <v>9678.7777582053113</v>
       </c>
       <c r="AC189" t="s">
         <v>132</v>

</xml_diff>